<commit_message>
Correct references in sources file
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848149F3-B28F-8D46-8DC1-D119477E6CC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C653C-B2D5-754E-94DB-D1604756A2ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28300" windowHeight="16700" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
   </bookViews>
@@ -2893,9 +2893,6 @@
     <t>REF_EU4</t>
   </si>
   <si>
-    <t>aiswal, K. S., and Wald, D. J. (2010b). Development of a semi-empirical loss model within the USGS Prompt Assessment of Global Earthquakes for Response (PAGER) System. Proc. of the 9th US and 10th Canadian Conference on Earthquake Engineering: Reaching Beyond Borders, July 25-29, 2010, Toronto, Canada. Available from URL: https://earthquake.usgs.gov/static/lfs/data/pager/Jaiswal_Wald_2010_Semi.pdf</t>
-  </si>
-  <si>
     <t>SERA Deliverable D26.3, Available from URL: http://eu-risk.eucentre.it/wp-content/uploads/2019/08/SERA_D26.3_Exposure_Models_Non-res_Res.pdf</t>
   </si>
   <si>
@@ -2924,6 +2921,9 @@
   </si>
   <si>
     <t>De Bono A, Chatenoux B (2014) A Global exposure model for GAR 2015. Available from URL: https://www.unisdr.org/we/inform/publications/49763.</t>
+  </si>
+  <si>
+    <t>Jaiswal, K. S., and Wald, D. J. (2010b). Development of a semi-empirical loss model within the USGS Prompt Assessment of Global Earthquakes for Response (PAGER) System. Proc. of the 9th US and 10th Canadian Conference on Earthquake Engineering: Reaching Beyond Borders, July 25-29, 2010, Toronto, Canada. Available from URL: https://earthquake.usgs.gov/static/lfs/data/pager/Jaiswal_Wald_2010_Semi.pdf</t>
   </si>
 </sst>
 </file>
@@ -3705,13 +3705,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3719,12 +3725,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4055,51 +4055,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="182" t="s">
         <v>901</v>
       </c>
-      <c r="B1" s="187"/>
+      <c r="B1" s="182"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="184" t="s">
+        <v>918</v>
+      </c>
+      <c r="B2" s="184"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="22" customHeight="1">
+      <c r="A3" s="186" t="s">
+        <v>920</v>
+      </c>
+      <c r="B3" s="184"/>
+    </row>
+    <row r="4" spans="1:3" ht="22" customHeight="1">
+      <c r="A4" s="184" t="s">
+        <v>900</v>
+      </c>
+      <c r="B4" s="184"/>
+    </row>
+    <row r="5" spans="1:3" ht="22" customHeight="1">
+      <c r="A5" s="184" t="s">
         <v>919</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="184" t="s">
-        <v>921</v>
-      </c>
-      <c r="B3" s="183"/>
-    </row>
-    <row r="4" spans="1:3" ht="22" customHeight="1">
-      <c r="A4" s="183" t="s">
-        <v>900</v>
-      </c>
-      <c r="B4" s="183"/>
-    </row>
-    <row r="5" spans="1:3" ht="22" customHeight="1">
-      <c r="A5" s="183" t="s">
-        <v>920</v>
-      </c>
-      <c r="B5" s="183"/>
+      <c r="B5" s="184"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="188"/>
-      <c r="B6" s="188"/>
+      <c r="A6" s="183"/>
+      <c r="B6" s="183"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="187" t="s">
         <v>692</v>
       </c>
-      <c r="B7" s="185"/>
+      <c r="B7" s="187"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="186" t="s">
+      <c r="A8" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="186"/>
+      <c r="B8" s="188"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4265,10 +4265,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="182" t="s">
+      <c r="A30" s="185" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="182"/>
+      <c r="B30" s="185"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4335,10 +4335,10 @@
       <c r="B39" s="4"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="182" t="s">
+      <c r="A41" s="185" t="s">
         <v>703</v>
       </c>
-      <c r="B41" s="182"/>
+      <c r="B41" s="185"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4357,16 +4357,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="185" t="s">
+      <c r="A45" s="187" t="s">
         <v>864</v>
       </c>
-      <c r="B45" s="185"/>
+      <c r="B45" s="187"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="186" t="s">
+      <c r="A46" s="188" t="s">
         <v>451</v>
       </c>
-      <c r="B46" s="186"/>
+      <c r="B46" s="188"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3"/>
@@ -4481,10 +4481,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="182" t="s">
+      <c r="A64" s="185" t="s">
         <v>703</v>
       </c>
-      <c r="B64" s="182"/>
+      <c r="B64" s="185"/>
     </row>
     <row r="65" spans="1:2" ht="51">
       <c r="A65" s="61" t="s">
@@ -4503,16 +4503,16 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="185" t="s">
+      <c r="A68" s="187" t="s">
         <v>863</v>
       </c>
-      <c r="B68" s="185"/>
+      <c r="B68" s="187"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="186" t="s">
+      <c r="A69" s="188" t="s">
         <v>551</v>
       </c>
-      <c r="B69" s="186"/>
+      <c r="B69" s="188"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3"/>
@@ -4595,10 +4595,10 @@
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="182" t="s">
+      <c r="A81" s="185" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="182"/>
+      <c r="B81" s="185"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4"/>
@@ -4637,10 +4637,10 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="182" t="s">
+      <c r="A88" s="185" t="s">
         <v>703</v>
       </c>
-      <c r="B88" s="182"/>
+      <c r="B88" s="185"/>
     </row>
     <row r="89" spans="1:2" ht="51">
       <c r="A89" s="61" t="s">
@@ -4668,12 +4668,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -4685,6 +4679,12 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13244,7 +13244,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13274,7 +13274,7 @@
         <v>898</v>
       </c>
       <c r="B3" s="136" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51">
@@ -13282,7 +13282,7 @@
         <v>903</v>
       </c>
       <c r="B4" s="136" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="51">
@@ -13290,7 +13290,7 @@
         <v>911</v>
       </c>
       <c r="B5" s="136" t="s">
-        <v>912</v>
+        <v>922</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -13302,7 +13302,7 @@
         <v>907</v>
       </c>
       <c r="B7" s="136" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -13314,7 +13314,7 @@
         <v>709</v>
       </c>
       <c r="B9" s="136" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34">
@@ -13330,7 +13330,7 @@
         <v>711</v>
       </c>
       <c r="B11" s="136" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="33" customHeight="1">
@@ -13338,7 +13338,7 @@
         <v>730</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13349,7 +13349,7 @@
         <v>763</v>
       </c>
       <c r="B14" s="181" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update link to Turkish residential data and date of Turkish population
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A64486-BBFE-A94E-B6DA-799E7DC03054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BC396A-0A68-334D-9C35-F3B25B2CAC8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
+    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="1" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="926">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -2927,6 +2927,15 @@
   </si>
   <si>
     <t>Sousa L., Silva V., and Bazzurro P. (2019) "Using Open-Access Data in the Development of Exposure Data Sets of Industrial Buildings for Earthquake Risk Modeling," Earthquake Spectra,  doi: https://doi.org/10.1193/020316eqs027m</t>
+  </si>
+  <si>
+    <t>Population and Housing Census (2017 value)
+https://data.tuik.gov.tr</t>
+  </si>
+  <si>
+    <t>2000 Population and Housing Census +
+2001-2017 Building permits
+https://data.tuik.gov.tr</t>
   </si>
 </sst>
 </file>
@@ -3711,13 +3720,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3725,12 +3740,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4050,7 +4059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDE1935-F182-8E4C-A9F6-BCE17C9647EE}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -4061,51 +4070,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="183" t="s">
         <v>896</v>
       </c>
-      <c r="B1" s="188"/>
+      <c r="B1" s="183"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="185" t="s">
         <v>912</v>
       </c>
-      <c r="B2" s="184"/>
+      <c r="B2" s="185"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="187" t="s">
         <v>914</v>
       </c>
-      <c r="B3" s="184"/>
+      <c r="B3" s="185"/>
     </row>
     <row r="4" spans="1:3" ht="22" customHeight="1">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="185" t="s">
         <v>895</v>
       </c>
-      <c r="B4" s="184"/>
+      <c r="B4" s="185"/>
     </row>
     <row r="5" spans="1:3" ht="22" customHeight="1">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="185" t="s">
         <v>913</v>
       </c>
-      <c r="B5" s="184"/>
+      <c r="B5" s="185"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="189"/>
-      <c r="B6" s="189"/>
+      <c r="A6" s="184"/>
+      <c r="B6" s="184"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="186" t="s">
+      <c r="A7" s="188" t="s">
         <v>688</v>
       </c>
-      <c r="B7" s="186"/>
+      <c r="B7" s="188"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="189" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="187"/>
+      <c r="B8" s="189"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4271,10 +4280,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="183" t="s">
+      <c r="A30" s="186" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="183"/>
+      <c r="B30" s="186"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4341,10 +4350,10 @@
       <c r="B39" s="4"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="183" t="s">
+      <c r="A41" s="186" t="s">
         <v>699</v>
       </c>
-      <c r="B41" s="183"/>
+      <c r="B41" s="186"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4363,16 +4372,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="186" t="s">
+      <c r="A45" s="188" t="s">
         <v>859</v>
       </c>
-      <c r="B45" s="186"/>
+      <c r="B45" s="188"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="187" t="s">
+      <c r="A46" s="189" t="s">
         <v>448</v>
       </c>
-      <c r="B46" s="187"/>
+      <c r="B46" s="189"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3"/>
@@ -4487,10 +4496,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="183" t="s">
+      <c r="A64" s="186" t="s">
         <v>699</v>
       </c>
-      <c r="B64" s="183"/>
+      <c r="B64" s="186"/>
     </row>
     <row r="65" spans="1:2" ht="51">
       <c r="A65" s="61" t="s">
@@ -4509,16 +4518,16 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="186" t="s">
+      <c r="A68" s="188" t="s">
         <v>858</v>
       </c>
-      <c r="B68" s="186"/>
+      <c r="B68" s="188"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="187" t="s">
+      <c r="A69" s="189" t="s">
         <v>547</v>
       </c>
-      <c r="B69" s="187"/>
+      <c r="B69" s="189"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3"/>
@@ -4601,10 +4610,10 @@
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="183" t="s">
+      <c r="A81" s="186" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="183"/>
+      <c r="B81" s="186"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4"/>
@@ -4643,10 +4652,10 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="183" t="s">
+      <c r="A88" s="186" t="s">
         <v>699</v>
       </c>
-      <c r="B88" s="183"/>
+      <c r="B88" s="186"/>
     </row>
     <row r="89" spans="1:2" ht="51">
       <c r="A89" s="61" t="s">
@@ -4674,12 +4683,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -4691,6 +4694,12 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4700,11 +4709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D9D520-21E0-4740-A733-1FA0F3F531E7}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AQ10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ17" sqref="AQ17"/>
+      <selection pane="bottomRight" activeCell="AR31" sqref="AR31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5483,7 +5492,7 @@
         <v>283</v>
       </c>
       <c r="AR6" s="22" t="s">
-        <v>286</v>
+        <v>925</v>
       </c>
       <c r="AS6" s="22" t="s">
         <v>900</v>
@@ -5757,7 +5766,7 @@
         <v>284</v>
       </c>
       <c r="AR8" s="7" t="s">
-        <v>287</v>
+        <v>924</v>
       </c>
       <c r="AS8" s="7" t="s">
         <v>288</v>
@@ -8554,7 +8563,7 @@
       </c>
       <c r="AP31" s="172"/>
       <c r="AQ31" s="172"/>
-      <c r="AR31" s="172"/>
+      <c r="AR31" s="174"/>
       <c r="AS31" s="172"/>
     </row>
     <row r="34" spans="1:10">

</xml_diff>

<commit_message>
Correct admin resolution levels for RES: Monaco, Isle of Man and Moldova
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38DD3BE3-C7CC-9942-A75F-F5167A302643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970E2A5-EDF6-3C48-9141-139FE529CE4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="28300" windowHeight="16700" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="28300" windowHeight="16700" activeTab="1" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -3700,13 +3700,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3714,15 +3723,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4042,7 +4042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDE1935-F182-8E4C-A9F6-BCE17C9647EE}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
@@ -4053,51 +4053,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="184" t="s">
         <v>894</v>
       </c>
-      <c r="B1" s="188"/>
+      <c r="B1" s="184"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="186" t="s">
         <v>911</v>
       </c>
-      <c r="B2" s="184"/>
+      <c r="B2" s="186"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="188" t="s">
         <v>913</v>
       </c>
-      <c r="B3" s="184"/>
+      <c r="B3" s="186"/>
     </row>
     <row r="4" spans="1:3" ht="22" customHeight="1">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="186" t="s">
         <v>893</v>
       </c>
-      <c r="B4" s="184"/>
+      <c r="B4" s="186"/>
     </row>
     <row r="5" spans="1:3" ht="22" customHeight="1">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="186" t="s">
         <v>912</v>
       </c>
-      <c r="B5" s="184"/>
+      <c r="B5" s="186"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="189"/>
-      <c r="B6" s="189"/>
+      <c r="A6" s="185"/>
+      <c r="B6" s="185"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="186" t="s">
+      <c r="A7" s="189" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="186"/>
+      <c r="B7" s="189"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="190" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="187"/>
+      <c r="B8" s="190"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4263,10 +4263,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="183" t="s">
+      <c r="A30" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="183"/>
+      <c r="B30" s="187"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4333,10 +4333,10 @@
       <c r="B39" s="4"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="183" t="s">
+      <c r="A41" s="187" t="s">
         <v>698</v>
       </c>
-      <c r="B41" s="183"/>
+      <c r="B41" s="187"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4355,16 +4355,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="186" t="s">
+      <c r="A45" s="189" t="s">
         <v>857</v>
       </c>
-      <c r="B45" s="186"/>
+      <c r="B45" s="189"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="187" t="s">
+      <c r="A46" s="190" t="s">
         <v>447</v>
       </c>
-      <c r="B46" s="187"/>
+      <c r="B46" s="190"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3"/>
@@ -4479,10 +4479,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="183" t="s">
+      <c r="A64" s="187" t="s">
         <v>698</v>
       </c>
-      <c r="B64" s="183"/>
+      <c r="B64" s="187"/>
     </row>
     <row r="65" spans="1:2" ht="51">
       <c r="A65" s="61" t="s">
@@ -4501,16 +4501,16 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="186" t="s">
+      <c r="A68" s="189" t="s">
         <v>856</v>
       </c>
-      <c r="B68" s="186"/>
+      <c r="B68" s="189"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="187" t="s">
+      <c r="A69" s="190" t="s">
         <v>546</v>
       </c>
-      <c r="B69" s="187"/>
+      <c r="B69" s="190"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3"/>
@@ -4593,10 +4593,10 @@
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="183" t="s">
+      <c r="A81" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="183"/>
+      <c r="B81" s="187"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4"/>
@@ -4635,10 +4635,10 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="183" t="s">
+      <c r="A88" s="187" t="s">
         <v>698</v>
       </c>
-      <c r="B88" s="183"/>
+      <c r="B88" s="187"/>
     </row>
     <row r="89" spans="1:2" ht="51">
       <c r="A89" s="61" t="s">
@@ -4666,12 +4666,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -4683,6 +4677,12 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4692,11 +4692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D9D520-21E0-4740-A733-1FA0F3F531E7}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5269,7 +5269,7 @@
         <v>34</v>
       </c>
       <c r="U5" s="51" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="V5" s="51" t="s">
         <v>35</v>
@@ -5293,10 +5293,10 @@
         <v>34</v>
       </c>
       <c r="AC5" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD5" s="51" t="s">
         <v>144</v>
-      </c>
-      <c r="AD5" s="51" t="s">
-        <v>34</v>
       </c>
       <c r="AE5" s="51" t="s">
         <v>34</v>
@@ -7366,7 +7366,7 @@
       <c r="AI20" s="43">
         <v>700</v>
       </c>
-      <c r="AJ20" s="190">
+      <c r="AJ20" s="183">
         <v>800</v>
       </c>
       <c r="AK20" s="43">

</xml_diff>

<commit_message>
update total dwellings in sources file (EuroStat 2011 data) for Malta, Italy, Luxembourg, Slovakia, Slovenia
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970E2A5-EDF6-3C48-9141-139FE529CE4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAE1857-253D-D94D-9E80-D3407C473479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="28300" windowHeight="16700" activeTab="1" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
+    <workbookView xWindow="2220" yWindow="460" windowWidth="28300" windowHeight="16700" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="924">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -3703,26 +3703,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4042,7 +4042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDE1935-F182-8E4C-A9F6-BCE17C9647EE}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
@@ -4053,51 +4053,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="189" t="s">
         <v>894</v>
       </c>
-      <c r="B1" s="184"/>
+      <c r="B1" s="189"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="185" t="s">
         <v>911</v>
       </c>
-      <c r="B2" s="186"/>
+      <c r="B2" s="185"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="188" t="s">
+      <c r="A3" s="186" t="s">
         <v>913</v>
       </c>
-      <c r="B3" s="186"/>
+      <c r="B3" s="185"/>
     </row>
     <row r="4" spans="1:3" ht="22" customHeight="1">
-      <c r="A4" s="186" t="s">
+      <c r="A4" s="185" t="s">
         <v>893</v>
       </c>
-      <c r="B4" s="186"/>
+      <c r="B4" s="185"/>
     </row>
     <row r="5" spans="1:3" ht="22" customHeight="1">
-      <c r="A5" s="186" t="s">
+      <c r="A5" s="185" t="s">
         <v>912</v>
       </c>
-      <c r="B5" s="186"/>
+      <c r="B5" s="185"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="185"/>
-      <c r="B6" s="185"/>
+      <c r="A6" s="190"/>
+      <c r="B6" s="190"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="189" t="s">
+      <c r="A7" s="187" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="187"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="190" t="s">
+      <c r="A8" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="190"/>
+      <c r="B8" s="188"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4263,10 +4263,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="187" t="s">
+      <c r="A30" s="184" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="187"/>
+      <c r="B30" s="184"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4333,10 +4333,10 @@
       <c r="B39" s="4"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="187" t="s">
+      <c r="A41" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B41" s="187"/>
+      <c r="B41" s="184"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4355,16 +4355,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="189" t="s">
+      <c r="A45" s="187" t="s">
         <v>857</v>
       </c>
-      <c r="B45" s="189"/>
+      <c r="B45" s="187"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="190" t="s">
+      <c r="A46" s="188" t="s">
         <v>447</v>
       </c>
-      <c r="B46" s="190"/>
+      <c r="B46" s="188"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3"/>
@@ -4479,10 +4479,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="187" t="s">
+      <c r="A64" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B64" s="187"/>
+      <c r="B64" s="184"/>
     </row>
     <row r="65" spans="1:2" ht="51">
       <c r="A65" s="61" t="s">
@@ -4501,16 +4501,16 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="189" t="s">
+      <c r="A68" s="187" t="s">
         <v>856</v>
       </c>
-      <c r="B68" s="189"/>
+      <c r="B68" s="187"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="190" t="s">
+      <c r="A69" s="188" t="s">
         <v>546</v>
       </c>
-      <c r="B69" s="190"/>
+      <c r="B69" s="188"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3"/>
@@ -4593,10 +4593,10 @@
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="187" t="s">
+      <c r="A81" s="184" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="187"/>
+      <c r="B81" s="184"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4"/>
@@ -4635,10 +4635,10 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="187" t="s">
+      <c r="A88" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B88" s="187"/>
+      <c r="B88" s="184"/>
     </row>
     <row r="89" spans="1:2" ht="51">
       <c r="A89" s="61" t="s">
@@ -4666,6 +4666,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -4677,12 +4683,6 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4692,11 +4692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D9D520-21E0-4740-A733-1FA0F3F531E7}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
+      <selection pane="bottomRight" activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8284,8 +8284,8 @@
       <c r="U28" s="20">
         <v>35599</v>
       </c>
-      <c r="V28" s="37" t="s">
-        <v>8</v>
+      <c r="V28" s="37">
+        <v>31208161</v>
       </c>
       <c r="W28" s="20">
         <v>412884</v>
@@ -8300,10 +8300,10 @@
         <v>1374233</v>
       </c>
       <c r="AA28" s="20">
-        <v>227326</v>
-      </c>
-      <c r="AB28" s="37" t="s">
-        <v>8</v>
+        <v>222946</v>
+      </c>
+      <c r="AB28" s="20">
+        <v>223850</v>
       </c>
       <c r="AC28" s="37" t="s">
         <v>8</v>
@@ -8333,11 +8333,11 @@
       <c r="AL28" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AM28" s="37" t="s">
-        <v>8</v>
+      <c r="AM28" s="20">
+        <v>194117</v>
       </c>
       <c r="AN28" s="20">
-        <v>777772</v>
+        <v>844656</v>
       </c>
       <c r="AO28" s="20">
         <v>25849338</v>
@@ -8417,8 +8417,8 @@
       <c r="U29" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="V29" s="38" t="s">
-        <v>8</v>
+      <c r="V29" s="182" t="s">
+        <v>921</v>
       </c>
       <c r="W29" s="55" t="s">
         <v>31</v>
@@ -8432,11 +8432,11 @@
       <c r="Z29" s="182" t="s">
         <v>921</v>
       </c>
-      <c r="AA29" s="55" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB29" s="38" t="s">
-        <v>8</v>
+      <c r="AA29" s="182" t="s">
+        <v>921</v>
+      </c>
+      <c r="AB29" s="182" t="s">
+        <v>921</v>
       </c>
       <c r="AC29" s="38" t="s">
         <v>8</v>
@@ -8466,11 +8466,11 @@
       <c r="AL29" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AM29" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN29" s="55" t="s">
-        <v>224</v>
+      <c r="AM29" s="182" t="s">
+        <v>921</v>
+      </c>
+      <c r="AN29" s="182" t="s">
+        <v>921</v>
       </c>
       <c r="AO29" s="55" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
update admin level for Luxembourg commercial
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D9B53A-BDB3-8749-A18D-5E2ADA8BCE34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9127CB8-B05C-9141-8472-44B4FB759C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="1" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
+    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="3" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -3709,29 +3709,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4062,10 +4062,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="189" t="s">
         <v>893</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="189"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
       <c r="A2" s="185" t="s">
@@ -4075,7 +4075,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="186" t="s">
         <v>912</v>
       </c>
       <c r="B3" s="185"/>
@@ -4093,20 +4093,20 @@
       <c r="B5" s="185"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="184"/>
-      <c r="B6" s="184"/>
+      <c r="A6" s="190"/>
+      <c r="B6" s="190"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="188" t="s">
+      <c r="A7" s="187" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="188"/>
+      <c r="B7" s="187"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="189" t="s">
+      <c r="A8" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="189"/>
+      <c r="B8" s="188"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4272,10 +4272,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="186" t="s">
+      <c r="A30" s="184" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="186"/>
+      <c r="B30" s="184"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4342,10 +4342,10 @@
       <c r="B39" s="4"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="186" t="s">
+      <c r="A41" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B41" s="186"/>
+      <c r="B41" s="184"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4364,16 +4364,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="188" t="s">
+      <c r="A45" s="187" t="s">
         <v>856</v>
       </c>
-      <c r="B45" s="188"/>
+      <c r="B45" s="187"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="189" t="s">
+      <c r="A46" s="188" t="s">
         <v>447</v>
       </c>
-      <c r="B46" s="189"/>
+      <c r="B46" s="188"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3"/>
@@ -4488,10 +4488,10 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="186" t="s">
+      <c r="A64" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B64" s="186"/>
+      <c r="B64" s="184"/>
     </row>
     <row r="65" spans="1:2" ht="51">
       <c r="A65" s="61" t="s">
@@ -4510,16 +4510,16 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="188" t="s">
+      <c r="A68" s="187" t="s">
         <v>855</v>
       </c>
-      <c r="B68" s="188"/>
+      <c r="B68" s="187"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="189" t="s">
+      <c r="A69" s="188" t="s">
         <v>546</v>
       </c>
-      <c r="B69" s="189"/>
+      <c r="B69" s="188"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3"/>
@@ -4602,10 +4602,10 @@
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="186" t="s">
+      <c r="A81" s="184" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="186"/>
+      <c r="B81" s="184"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4"/>
@@ -4644,10 +4644,10 @@
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="186" t="s">
+      <c r="A88" s="184" t="s">
         <v>698</v>
       </c>
-      <c r="B88" s="186"/>
+      <c r="B88" s="184"/>
     </row>
     <row r="89" spans="1:2" ht="51">
       <c r="A89" s="61" t="s">
@@ -4675,6 +4675,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -4686,12 +4692,6 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4701,7 +4701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D9D520-21E0-4740-A733-1FA0F3F531E7}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8535,7 +8535,7 @@
       <c r="Y31" s="170"/>
       <c r="Z31" s="170"/>
       <c r="AA31" s="170"/>
-      <c r="AB31" s="190" t="s">
+      <c r="AB31" s="183" t="s">
         <v>926</v>
       </c>
       <c r="AC31" s="172" t="s">
@@ -8552,7 +8552,7 @@
       </c>
       <c r="AK31" s="170"/>
       <c r="AL31" s="170"/>
-      <c r="AM31" s="190" t="s">
+      <c r="AM31" s="183" t="s">
         <v>925</v>
       </c>
       <c r="AN31" s="170"/>
@@ -10987,11 +10987,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AEA308-1482-084B-80EE-660006D8760C}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U11" sqref="U11"/>
+      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11676,7 +11676,7 @@
         <v>34</v>
       </c>
       <c r="AA6" s="94" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="AB6" s="94" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
changed format of ratios in the Notes tab of European_Exposure_Model_Data_Inputs_Sources.xlsx
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\GFZ_local\SERA\From_EFEHR_GitLab\esrm20_exposure\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9127CB8-B05C-9141-8472-44B4FB759C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="3" xr2:uid="{3ADB8CE8-CD4D-1C4D-B72A-BA24B45CE5E7}"/>
+    <workbookView xWindow="504" yWindow="516" windowWidth="28296" windowHeight="16704"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="COM" sheetId="2" r:id="rId4"/>
     <sheet name="References" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="932">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -2664,9 +2663,6 @@
     <t>Population spatial distribution data</t>
   </si>
   <si>
-    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 80% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the following percentages: 0.3, 0.5, 0.2, respectively. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
-  </si>
-  <si>
     <t>Change in CDL lateral force coefficients not considered (due to year not being in mapping scheme)</t>
   </si>
   <si>
@@ -2731,12 +2727,6 @@
   </si>
   <si>
     <t>Occupants (day, night, transit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 40% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the following percentages: 0.15, 0.25, 0.6, respectively. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 50% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the following percentages: 0.2, 0.3, 0.5, respectively. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
   </si>
   <si>
     <t>Name of the file that contains the mapping scheme to map census attributes to bulding classes (inside folder 'res_mapping_schemes')</t>
@@ -2936,17 +2926,41 @@
   </si>
   <si>
     <t>The dwellings from the 2005 census have been uniformly scaled to the total number of dwellings from Eurostat 2011</t>
+  </si>
+  <si>
+    <t>Occupants</t>
+  </si>
+  <si>
+    <t>Replacement cost: structural / total</t>
+  </si>
+  <si>
+    <t>Replacement cost: non-structural / total</t>
+  </si>
+  <si>
+    <t>Replacement cost: contents / total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 80% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the percentages shown in the rows below. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
+  </si>
+  <si>
+    <t>Replacement Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 40% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the percentages shown in the rows below. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 50% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the percentages shown in the rows below. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3013,6 +3027,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3237,9 +3263,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3607,7 +3633,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3712,13 +3738,19 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3727,11 +3759,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4048,65 +4086,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDE1935-F182-8E4C-A9F6-BCE17C9647EE}">
-  <dimension ref="A1:D91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="155.6640625" customWidth="1"/>
+    <col min="1" max="1" width="44.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="155.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="189" t="s">
-        <v>893</v>
-      </c>
-      <c r="B1" s="189"/>
-    </row>
-    <row r="2" spans="1:3" ht="22" customHeight="1">
-      <c r="A2" s="185" t="s">
-        <v>910</v>
-      </c>
-      <c r="B2" s="185"/>
+      <c r="A1" s="184" t="s">
+        <v>890</v>
+      </c>
+      <c r="B1" s="184"/>
+    </row>
+    <row r="2" spans="1:3" ht="22.05" customHeight="1">
+      <c r="A2" s="186" t="s">
+        <v>907</v>
+      </c>
+      <c r="B2" s="186"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="186" t="s">
-        <v>912</v>
-      </c>
-      <c r="B3" s="185"/>
-    </row>
-    <row r="4" spans="1:3" ht="22" customHeight="1">
-      <c r="A4" s="185" t="s">
-        <v>892</v>
-      </c>
-      <c r="B4" s="185"/>
-    </row>
-    <row r="5" spans="1:3" ht="22" customHeight="1">
-      <c r="A5" s="185" t="s">
-        <v>911</v>
-      </c>
-      <c r="B5" s="185"/>
+    <row r="3" spans="1:3" ht="22.05" customHeight="1">
+      <c r="A3" s="188" t="s">
+        <v>909</v>
+      </c>
+      <c r="B3" s="186"/>
+    </row>
+    <row r="4" spans="1:3" ht="22.05" customHeight="1">
+      <c r="A4" s="186" t="s">
+        <v>889</v>
+      </c>
+      <c r="B4" s="186"/>
+    </row>
+    <row r="5" spans="1:3" ht="22.05" customHeight="1">
+      <c r="A5" s="186" t="s">
+        <v>908</v>
+      </c>
+      <c r="B5" s="186"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="190"/>
-      <c r="B6" s="190"/>
-    </row>
-    <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="187" t="s">
+      <c r="A6" s="185"/>
+      <c r="B6" s="185"/>
+    </row>
+    <row r="7" spans="1:3" ht="38.4">
+      <c r="A7" s="189" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="187"/>
+      <c r="B7" s="189"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="188" t="s">
+      <c r="A8" s="190" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="188"/>
+      <c r="B8" s="190"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4149,7 +4187,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4165,7 +4203,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4248,7 +4286,7 @@
         <v>827</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4256,7 +4294,7 @@
         <v>828</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4264,7 +4302,7 @@
         <v>829</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4272,10 +4310,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="184" t="s">
+      <c r="A30" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="184"/>
+      <c r="B30" s="187"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4337,368 +4375,465 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="184" t="s">
-        <v>698</v>
-      </c>
-      <c r="B41" s="184"/>
-    </row>
-    <row r="42" spans="1:2" ht="51">
+    <row r="40" spans="1:2">
+      <c r="A40" s="191" t="s">
+        <v>929</v>
+      </c>
+      <c r="B40" s="191"/>
+    </row>
+    <row r="42" spans="1:2" ht="46.8">
       <c r="A42" s="61" t="s">
         <v>830</v>
       </c>
-      <c r="B42" s="68" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="34">
-      <c r="A43" s="8" t="s">
-        <v>858</v>
-      </c>
-      <c r="B43" s="174" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="39">
-      <c r="A45" s="187" t="s">
-        <v>856</v>
-      </c>
-      <c r="B45" s="187"/>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="188" t="s">
+      <c r="B42" s="193" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="192" t="s">
+        <v>925</v>
+      </c>
+      <c r="B43" s="194">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="192" t="s">
+        <v>926</v>
+      </c>
+      <c r="B44" s="194">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="192" t="s">
+        <v>927</v>
+      </c>
+      <c r="B45" s="194">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="191" t="s">
+        <v>924</v>
+      </c>
+      <c r="B47" s="191"/>
+    </row>
+    <row r="49" spans="1:2" ht="31.2">
+      <c r="A49" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="B49" s="174" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="38.4">
+      <c r="A51" s="189" t="s">
+        <v>855</v>
+      </c>
+      <c r="B51" s="189"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="190" t="s">
         <v>447</v>
       </c>
-      <c r="B46" s="188"/>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="91" t="s">
+      <c r="B52" s="190"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="91" t="s">
         <v>448</v>
       </c>
-      <c r="B48" s="91"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="66" t="s">
+      <c r="B54" s="91"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="66" t="s">
         <v>449</v>
       </c>
-      <c r="B49" s="66"/>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="66" t="s">
+      <c r="B55" s="66"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="66" t="s">
         <v>450</v>
       </c>
-      <c r="B50" s="66"/>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="66" t="s">
+      <c r="B56" s="66"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="66" t="s">
         <v>451</v>
       </c>
-      <c r="B51" s="66"/>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="92" t="s">
+      <c r="B57" s="66"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="102" t="s">
+      <c r="B58" s="18" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="102" t="s">
         <v>460</v>
       </c>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="103" t="s">
+      <c r="B59" s="6"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="148"/>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="90" t="s">
+      <c r="B60" s="148"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="90" t="s">
         <v>723</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B61" s="13" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="90" t="s">
+        <v>452</v>
+      </c>
+      <c r="B62" s="82" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="10" t="s">
+        <v>712</v>
+      </c>
+      <c r="B64" s="10" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="90" t="s">
-        <v>452</v>
-      </c>
-      <c r="B56" s="82" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="41" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="90" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="175" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="125" t="s">
+        <v>830</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="191" t="s">
+        <v>929</v>
+      </c>
+      <c r="B70" s="191"/>
+    </row>
+    <row r="72" spans="1:2" ht="46.8">
+      <c r="A72" s="61" t="s">
+        <v>830</v>
+      </c>
+      <c r="B72" s="68" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="192" t="s">
+        <v>925</v>
+      </c>
+      <c r="B73" s="194">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="192" t="s">
+        <v>926</v>
+      </c>
+      <c r="B74" s="194">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="192" t="s">
+        <v>927</v>
+      </c>
+      <c r="B75" s="194">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="191" t="s">
+        <v>924</v>
+      </c>
+      <c r="B77" s="191"/>
+    </row>
+    <row r="79" spans="1:2" ht="31.2">
+      <c r="A79" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="B79" s="174" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="38.4">
+      <c r="A81" s="189" t="s">
+        <v>854</v>
+      </c>
+      <c r="B81" s="189"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="190" t="s">
+        <v>546</v>
+      </c>
+      <c r="B82" s="190"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" ht="31.2">
+      <c r="A84" s="151" t="s">
+        <v>776</v>
+      </c>
+      <c r="B84" s="151" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="152" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="109" t="s">
+        <v>708</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="175" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="155" t="s">
+        <v>833</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="130" t="s">
+        <v>832</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="156" t="s">
+        <v>831</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="187" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94" s="187"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="139" t="s">
+        <v>869</v>
+      </c>
+      <c r="B96" s="139" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="138" t="s">
+        <v>871</v>
+      </c>
+      <c r="B97" s="138" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="138" t="s">
+        <v>870</v>
+      </c>
+      <c r="B98" s="138" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="14" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="10" t="s">
-        <v>712</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="41" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="82" t="s">
+      <c r="B99" s="36" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="191" t="s">
+        <v>929</v>
+      </c>
+      <c r="B101" s="191"/>
+    </row>
+    <row r="103" spans="1:2" ht="46.8">
+      <c r="A103" s="61" t="s">
+        <v>830</v>
+      </c>
+      <c r="B103" s="68" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="192" t="s">
+        <v>925</v>
+      </c>
+      <c r="B104" s="194">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="192" t="s">
+        <v>926</v>
+      </c>
+      <c r="B105" s="194">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="192" t="s">
+        <v>927</v>
+      </c>
+      <c r="B106" s="194">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="191" t="s">
+        <v>924</v>
+      </c>
+      <c r="B108" s="191"/>
+    </row>
+    <row r="110" spans="1:2" ht="31.2">
+      <c r="A110" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="B110" s="174" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="187" t="s">
+        <v>698</v>
+      </c>
+      <c r="B112" s="187"/>
+    </row>
+    <row r="114" spans="1:2" ht="31.2" customHeight="1">
+      <c r="A114" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="175" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="125" t="s">
-        <v>830</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="184" t="s">
-        <v>698</v>
-      </c>
-      <c r="B64" s="184"/>
-    </row>
-    <row r="65" spans="1:2" ht="51">
-      <c r="A65" s="61" t="s">
-        <v>830</v>
-      </c>
-      <c r="B65" s="68" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="34">
-      <c r="A66" s="8" t="s">
-        <v>858</v>
-      </c>
-      <c r="B66" s="174" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="39">
-      <c r="A68" s="187" t="s">
-        <v>855</v>
-      </c>
-      <c r="B68" s="187"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="188" t="s">
-        <v>546</v>
-      </c>
-      <c r="B69" s="188"/>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="34">
-      <c r="A71" s="151" t="s">
-        <v>776</v>
-      </c>
-      <c r="B71" s="151" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="152" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="109" t="s">
-        <v>708</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" s="41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="128" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="175" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="6" t="s">
-        <v>549</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="155" t="s">
-        <v>833</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="130" t="s">
-        <v>832</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="156" t="s">
-        <v>831</v>
-      </c>
-      <c r="B79" s="18" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="184" t="s">
-        <v>212</v>
-      </c>
-      <c r="B81" s="184"/>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="139" t="s">
-        <v>872</v>
-      </c>
-      <c r="B83" s="139" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="138" t="s">
-        <v>874</v>
-      </c>
-      <c r="B84" s="138" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="138" t="s">
-        <v>873</v>
-      </c>
-      <c r="B85" s="138" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="184" t="s">
-        <v>698</v>
-      </c>
-      <c r="B88" s="184"/>
-    </row>
-    <row r="89" spans="1:2" ht="51">
-      <c r="A89" s="61" t="s">
-        <v>830</v>
-      </c>
-      <c r="B89" s="68" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="34">
-      <c r="A90" s="8" t="s">
-        <v>858</v>
-      </c>
-      <c r="B90" s="174" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="51">
-      <c r="A91" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B91" s="68" t="s">
-        <v>864</v>
+      <c r="B114" s="68" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A77:B77"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D9D520-21E0-4740-A733-1FA0F3F531E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4708,55 +4843,55 @@
       <selection pane="bottomRight" activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="41" style="28" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.296875" customWidth="1"/>
+    <col min="7" max="7" width="61.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.296875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" customWidth="1"/>
     <col min="16" max="16" width="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="37.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="37" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.83203125" customWidth="1"/>
+    <col min="20" max="20" width="35.796875" customWidth="1"/>
     <col min="21" max="21" width="36" customWidth="1"/>
-    <col min="22" max="22" width="34.83203125" customWidth="1"/>
+    <col min="22" max="22" width="34.796875" customWidth="1"/>
     <col min="23" max="23" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.83203125" customWidth="1"/>
-    <col min="25" max="25" width="40.1640625" customWidth="1"/>
-    <col min="26" max="26" width="37.33203125" customWidth="1"/>
-    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.33203125" customWidth="1"/>
-    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.1640625" customWidth="1"/>
-    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.796875" customWidth="1"/>
+    <col min="25" max="25" width="40.19921875" customWidth="1"/>
+    <col min="26" max="26" width="37.296875" customWidth="1"/>
+    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.296875" customWidth="1"/>
+    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.19921875" customWidth="1"/>
+    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.296875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="39.6640625" customWidth="1"/>
-    <col min="35" max="35" width="45.6640625" customWidth="1"/>
-    <col min="36" max="36" width="40.6640625" customWidth="1"/>
-    <col min="37" max="37" width="55.1640625" customWidth="1"/>
-    <col min="38" max="38" width="41.83203125" customWidth="1"/>
-    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="39.69921875" customWidth="1"/>
+    <col min="35" max="35" width="45.69921875" customWidth="1"/>
+    <col min="36" max="36" width="40.69921875" customWidth="1"/>
+    <col min="37" max="37" width="55.19921875" customWidth="1"/>
+    <col min="38" max="38" width="41.796875" customWidth="1"/>
+    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.83203125" customWidth="1"/>
-    <col min="43" max="43" width="59.6640625" customWidth="1"/>
-    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.796875" customWidth="1"/>
+    <col min="43" max="43" width="59.69921875" customWidth="1"/>
+    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -4893,7 +5028,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="2" spans="1:45" s="1" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
@@ -5353,7 +5488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="51">
+    <row r="6" spans="1:45" ht="46.8">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -5361,7 +5496,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>42</v>
@@ -5382,16 +5517,16 @@
         <v>118</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="N6" s="72" t="s">
         <v>133</v>
@@ -5400,7 +5535,7 @@
         <v>139</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Q6" s="22" t="s">
         <v>150</v>
@@ -5412,10 +5547,10 @@
         <v>161</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="V6" s="22" t="s">
         <v>823</v>
@@ -5424,16 +5559,16 @@
         <v>175</v>
       </c>
       <c r="X6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Y6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Z6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AA6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AB6" s="22" t="s">
         <v>194</v>
@@ -5442,7 +5577,7 @@
         <v>199</v>
       </c>
       <c r="AD6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AE6" s="22" t="s">
         <v>206</v>
@@ -5457,7 +5592,7 @@
         <v>229</v>
       </c>
       <c r="AI6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AJ6" s="22" t="s">
         <v>240</v>
@@ -5478,7 +5613,7 @@
         <v>273</v>
       </c>
       <c r="AP6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AQ6" s="22" t="s">
         <v>282</v>
@@ -5487,7 +5622,7 @@
         <v>285</v>
       </c>
       <c r="AS6" s="22" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -5627,7 +5762,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="34">
+    <row r="8" spans="1:45" ht="31.2">
       <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
@@ -5635,7 +5770,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>31</v>
@@ -5674,7 +5809,7 @@
         <v>31</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Q8" s="7" t="s">
         <v>31</v>
@@ -5689,7 +5824,7 @@
         <v>168</v>
       </c>
       <c r="U8" s="76" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="V8" s="76" t="s">
         <v>31</v>
@@ -5701,7 +5836,7 @@
         <v>181</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Z8" s="7" t="s">
         <v>188</v>
@@ -5716,7 +5851,7 @@
         <v>201</v>
       </c>
       <c r="AD8" s="7" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AE8" s="7" t="s">
         <v>31</v>
@@ -6312,111 +6447,111 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="17">
+    <row r="13" spans="1:45">
       <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="J13" s="73" t="s">
+        <v>893</v>
+      </c>
+      <c r="K13" s="73" t="s">
+        <v>893</v>
+      </c>
+      <c r="L13" s="73" t="s">
+        <v>893</v>
+      </c>
+      <c r="M13" s="73" t="s">
+        <v>893</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>893</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="T13" s="14" t="s">
+        <v>893</v>
+      </c>
+      <c r="U13" s="14" t="s">
         <v>894</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="J13" s="73" t="s">
-        <v>896</v>
-      </c>
-      <c r="K13" s="73" t="s">
-        <v>896</v>
-      </c>
-      <c r="L13" s="73" t="s">
-        <v>896</v>
-      </c>
-      <c r="M13" s="73" t="s">
-        <v>896</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="O13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>896</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="R13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="S13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="T13" s="14" t="s">
-        <v>896</v>
-      </c>
-      <c r="U13" s="14" t="s">
-        <v>897</v>
       </c>
       <c r="V13" s="14" t="s">
         <v>243</v>
       </c>
       <c r="W13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="X13" s="22" t="s">
         <v>894</v>
       </c>
-      <c r="X13" s="22" t="s">
-        <v>897</v>
-      </c>
       <c r="Y13" s="14" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Z13" s="22" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AA13" s="22" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AB13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AC13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AD13" s="14" t="s">
+        <v>893</v>
+      </c>
+      <c r="AE13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AF13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AG13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AH13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AI13" s="22" t="s">
         <v>894</v>
-      </c>
-      <c r="AC13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AD13" s="14" t="s">
-        <v>896</v>
-      </c>
-      <c r="AE13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AF13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AG13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AH13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AI13" s="22" t="s">
-        <v>897</v>
       </c>
       <c r="AJ13" s="14" t="s">
         <v>249</v>
@@ -6428,25 +6563,25 @@
         <v>259</v>
       </c>
       <c r="AM13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AN13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AO13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AP13" s="22" t="s">
         <v>894</v>
       </c>
-      <c r="AN13" s="14" t="s">
+      <c r="AQ13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AR13" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="AS13" s="14" t="s">
         <v>894</v>
-      </c>
-      <c r="AO13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AP13" s="22" t="s">
-        <v>897</v>
-      </c>
-      <c r="AQ13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AR13" s="14" t="s">
-        <v>894</v>
-      </c>
-      <c r="AS13" s="14" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -6454,28 +6589,28 @@
         <v>9</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>406</v>
@@ -6490,22 +6625,22 @@
         <v>406</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="Q14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="T14" s="11" t="s">
         <v>406</v>
@@ -6514,10 +6649,10 @@
         <v>406</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="W14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="X14" s="11" t="s">
         <v>406</v>
@@ -6541,13 +6676,13 @@
         <v>406</v>
       </c>
       <c r="AE14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AF14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="AG14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AH14" s="11" t="s">
         <v>406</v>
@@ -6556,31 +6691,31 @@
         <v>406</v>
       </c>
       <c r="AJ14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AK14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AL14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AM14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="AN14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AO14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AP14" s="11" t="s">
         <v>406</v>
       </c>
       <c r="AQ14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AR14" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="AS14" s="11" t="s">
         <v>406</v>
@@ -6731,7 +6866,7 @@
         <v>108</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>47</v>
@@ -6752,16 +6887,16 @@
         <v>108</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>136</v>
@@ -6770,7 +6905,7 @@
         <v>141</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Q16" s="9" t="s">
         <v>108</v>
@@ -6782,10 +6917,10 @@
         <v>205</v>
       </c>
       <c r="T16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="U16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="V16" s="78" t="s">
         <v>826</v>
@@ -6794,16 +6929,16 @@
         <v>177</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Y16" s="9" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Z16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AA16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AB16" s="9" t="s">
         <v>197</v>
@@ -6812,7 +6947,7 @@
         <v>136</v>
       </c>
       <c r="AD16" s="9" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="AE16" s="74" t="s">
         <v>269</v>
@@ -6846,7 +6981,7 @@
         <v>276</v>
       </c>
       <c r="AP16" s="9" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="AQ16" s="74" t="s">
         <v>292</v>
@@ -6855,10 +6990,10 @@
         <v>294</v>
       </c>
       <c r="AS16" s="9" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="17" spans="1:45" ht="191" customHeight="1">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" ht="190.95" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>13</v>
       </c>
@@ -6923,7 +7058,7 @@
         <v>403</v>
       </c>
       <c r="V17" s="61" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="W17" s="61" t="s">
         <v>179</v>
@@ -6965,10 +7100,10 @@
         <v>403</v>
       </c>
       <c r="AJ17" s="79" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="AK17" s="79" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="AL17" s="84" t="s">
         <v>441</v>
@@ -6977,7 +7112,7 @@
         <v>255</v>
       </c>
       <c r="AN17" s="86" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="AO17" s="61" t="s">
         <v>277</v>
@@ -7685,7 +7820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:45" ht="153">
+    <row r="24" spans="1:45" ht="140.4">
       <c r="A24" s="25" t="s">
         <v>12</v>
       </c>
@@ -7822,7 +7957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:45" ht="34">
+    <row r="25" spans="1:45" ht="31.2">
       <c r="A25" s="27" t="s">
         <v>2</v>
       </c>
@@ -8094,7 +8229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:45" ht="34">
+    <row r="27" spans="1:45" ht="31.2">
       <c r="A27" s="24" t="s">
         <v>2</v>
       </c>
@@ -8362,7 +8497,7 @@
         <v>22900000</v>
       </c>
     </row>
-    <row r="29" spans="1:45" ht="34">
+    <row r="29" spans="1:45" ht="31.2">
       <c r="A29" s="36" t="s">
         <v>2</v>
       </c>
@@ -8394,13 +8529,13 @@
         <v>122</v>
       </c>
       <c r="K29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="L29" s="55" t="s">
         <v>31</v>
       </c>
       <c r="M29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="N29" s="38" t="s">
         <v>8</v>
@@ -8415,19 +8550,19 @@
         <v>31</v>
       </c>
       <c r="R29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="S29" s="38" t="s">
         <v>8</v>
       </c>
       <c r="T29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="U29" s="55" t="s">
         <v>679</v>
       </c>
       <c r="V29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="W29" s="55" t="s">
         <v>31</v>
@@ -8439,13 +8574,13 @@
         <v>680</v>
       </c>
       <c r="Z29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AA29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AB29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AC29" s="38" t="s">
         <v>8</v>
@@ -8464,7 +8599,7 @@
         <v>8</v>
       </c>
       <c r="AI29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AJ29" s="55" t="s">
         <v>31</v>
@@ -8476,16 +8611,16 @@
         <v>8</v>
       </c>
       <c r="AM29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AN29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AO29" s="55" t="s">
         <v>31</v>
       </c>
       <c r="AP29" s="181" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AQ29" s="55" t="s">
         <v>283</v>
@@ -8495,7 +8630,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:45" s="4" customFormat="1" ht="130" customHeight="1">
+    <row r="31" spans="1:45" s="4" customFormat="1" ht="130.05000000000001" customHeight="1">
       <c r="A31" s="67" t="s">
         <v>138</v>
       </c>
@@ -8507,7 +8642,7 @@
       <c r="G31" s="170"/>
       <c r="H31" s="19"/>
       <c r="I31" s="171" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="J31" s="170"/>
       <c r="K31" s="170"/>
@@ -8520,26 +8655,26 @@
       <c r="P31" s="170"/>
       <c r="Q31" s="170"/>
       <c r="R31" s="172" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="S31" s="170"/>
       <c r="T31" s="170"/>
       <c r="U31" s="170"/>
       <c r="V31" s="171" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="W31" s="171" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="X31" s="170"/>
       <c r="Y31" s="170"/>
       <c r="Z31" s="170"/>
       <c r="AA31" s="170"/>
       <c r="AB31" s="183" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="AC31" s="172" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="AD31" s="170"/>
       <c r="AE31" s="170"/>
@@ -8548,16 +8683,16 @@
       <c r="AH31" s="19"/>
       <c r="AI31" s="170"/>
       <c r="AJ31" s="172" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="AK31" s="170"/>
       <c r="AL31" s="170"/>
       <c r="AM31" s="183" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="AN31" s="170"/>
       <c r="AO31" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AP31" s="170"/>
       <c r="AQ31" s="170"/>
@@ -8706,9 +8841,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F25" r:id="rId1" xr:uid="{FCA6F18E-1626-134B-8756-FBE4351EDE74}"/>
-    <hyperlink ref="F27" r:id="rId2" xr:uid="{FF0F616F-5433-744C-A5FC-8EBF552F493F}"/>
-    <hyperlink ref="F29" r:id="rId3" xr:uid="{68C4F114-6133-F049-9B01-9A4B54FDD220}"/>
+    <hyperlink ref="F25" r:id="rId1"/>
+    <hyperlink ref="F27" r:id="rId2"/>
+    <hyperlink ref="F29" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8716,7 +8851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E556547C-C132-9D4F-8892-5C1D16968525}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8726,56 +8861,56 @@
       <selection pane="bottomRight" activeCell="AS17" sqref="B17:AS17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.296875" customWidth="1"/>
+    <col min="4" max="4" width="35.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.5" customWidth="1"/>
-    <col min="8" max="8" width="48.83203125" customWidth="1"/>
+    <col min="8" max="8" width="48.796875" customWidth="1"/>
     <col min="9" max="9" width="43.5" customWidth="1"/>
-    <col min="10" max="10" width="47.83203125" customWidth="1"/>
-    <col min="11" max="11" width="46.33203125" customWidth="1"/>
-    <col min="12" max="12" width="44.1640625" customWidth="1"/>
-    <col min="13" max="13" width="44.33203125" customWidth="1"/>
-    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="47.1640625" customWidth="1"/>
+    <col min="10" max="10" width="47.796875" customWidth="1"/>
+    <col min="11" max="11" width="46.296875" customWidth="1"/>
+    <col min="12" max="12" width="44.19921875" customWidth="1"/>
+    <col min="13" max="13" width="44.296875" customWidth="1"/>
+    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.19921875" customWidth="1"/>
     <col min="16" max="16" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41" customWidth="1"/>
     <col min="20" max="20" width="41.5" customWidth="1"/>
-    <col min="21" max="21" width="43.83203125" customWidth="1"/>
-    <col min="22" max="22" width="34.83203125" customWidth="1"/>
+    <col min="21" max="21" width="43.796875" customWidth="1"/>
+    <col min="22" max="22" width="34.796875" customWidth="1"/>
     <col min="23" max="23" width="39" customWidth="1"/>
-    <col min="24" max="24" width="37.83203125" customWidth="1"/>
-    <col min="25" max="25" width="40.1640625" customWidth="1"/>
-    <col min="26" max="26" width="37.33203125" customWidth="1"/>
-    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.33203125" customWidth="1"/>
-    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.1640625" customWidth="1"/>
-    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.796875" customWidth="1"/>
+    <col min="25" max="25" width="40.19921875" customWidth="1"/>
+    <col min="26" max="26" width="37.296875" customWidth="1"/>
+    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.296875" customWidth="1"/>
+    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.19921875" customWidth="1"/>
+    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.296875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="39.6640625" customWidth="1"/>
-    <col min="35" max="35" width="45.6640625" customWidth="1"/>
-    <col min="36" max="36" width="39.1640625" customWidth="1"/>
+    <col min="34" max="34" width="39.69921875" customWidth="1"/>
+    <col min="35" max="35" width="45.69921875" customWidth="1"/>
+    <col min="36" max="36" width="39.19921875" customWidth="1"/>
     <col min="37" max="37" width="40" customWidth="1"/>
-    <col min="38" max="38" width="41.83203125" customWidth="1"/>
-    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="41.796875" customWidth="1"/>
+    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.83203125" customWidth="1"/>
-    <col min="43" max="43" width="59.6640625" customWidth="1"/>
-    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.796875" customWidth="1"/>
+    <col min="43" max="43" width="59.69921875" customWidth="1"/>
+    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -9429,7 +9564,7 @@
         <v>201200</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="68">
+    <row r="7" spans="1:45" ht="62.4">
       <c r="A7" s="92" t="s">
         <v>2</v>
       </c>
@@ -9693,7 +9828,7 @@
         <v>201200</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="85">
+    <row r="9" spans="1:45" ht="78">
       <c r="A9" s="103" t="s">
         <v>2</v>
       </c>
@@ -10231,7 +10366,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="13" spans="1:45" s="4" customFormat="1" ht="51">
+    <row r="13" spans="1:45" s="4" customFormat="1" ht="46.8">
       <c r="A13" s="10" t="s">
         <v>712</v>
       </c>
@@ -10916,7 +11051,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="19" spans="1:45" s="123" customFormat="1" ht="34">
+    <row r="19" spans="1:45" s="123" customFormat="1" ht="31.2">
       <c r="A19" s="159" t="s">
         <v>138</v>
       </c>
@@ -10928,7 +11063,7 @@
       <c r="G19" s="166"/>
       <c r="H19" s="162"/>
       <c r="I19" s="163" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J19" s="162"/>
       <c r="K19" s="162"/>
@@ -10950,7 +11085,7 @@
       <c r="AA19" s="163"/>
       <c r="AB19" s="163"/>
       <c r="AC19" s="163" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="AD19" s="163"/>
       <c r="AE19" s="163"/>
@@ -10959,14 +11094,14 @@
       <c r="AH19" s="163"/>
       <c r="AI19" s="163"/>
       <c r="AJ19" s="163" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="AK19" s="163"/>
       <c r="AL19" s="164"/>
       <c r="AM19" s="164"/>
       <c r="AN19" s="164"/>
       <c r="AO19" s="163" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="AP19" s="164"/>
       <c r="AQ19" s="164"/>
@@ -10984,66 +11119,66 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AEA308-1482-084B-80EE-660006D8760C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.33203125" customWidth="1"/>
-    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.33203125" customWidth="1"/>
-    <col min="8" max="8" width="48.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.296875" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.296875" customWidth="1"/>
+    <col min="4" max="4" width="47.796875" customWidth="1"/>
+    <col min="5" max="5" width="59.296875" customWidth="1"/>
+    <col min="6" max="6" width="49.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.296875" customWidth="1"/>
+    <col min="8" max="8" width="48.796875" customWidth="1"/>
     <col min="9" max="9" width="43.5" customWidth="1"/>
-    <col min="10" max="10" width="47.83203125" customWidth="1"/>
-    <col min="11" max="11" width="46.33203125" customWidth="1"/>
-    <col min="12" max="12" width="44.1640625" customWidth="1"/>
-    <col min="13" max="13" width="44.33203125" customWidth="1"/>
-    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.796875" customWidth="1"/>
+    <col min="11" max="11" width="46.296875" customWidth="1"/>
+    <col min="12" max="12" width="44.19921875" customWidth="1"/>
+    <col min="13" max="13" width="44.296875" customWidth="1"/>
+    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="50" customWidth="1"/>
     <col min="16" max="16" width="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="60.83203125" customWidth="1"/>
+    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="60.796875" customWidth="1"/>
     <col min="19" max="19" width="43.5" customWidth="1"/>
-    <col min="20" max="20" width="49.1640625" customWidth="1"/>
+    <col min="20" max="20" width="49.19921875" customWidth="1"/>
     <col min="21" max="21" width="36" customWidth="1"/>
-    <col min="22" max="22" width="34.83203125" customWidth="1"/>
-    <col min="23" max="23" width="55.33203125" customWidth="1"/>
-    <col min="24" max="24" width="43.83203125" customWidth="1"/>
-    <col min="25" max="25" width="40.1640625" customWidth="1"/>
-    <col min="26" max="26" width="37.33203125" customWidth="1"/>
-    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.33203125" customWidth="1"/>
-    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.1640625" customWidth="1"/>
-    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="56.33203125" customWidth="1"/>
+    <col min="22" max="22" width="34.796875" customWidth="1"/>
+    <col min="23" max="23" width="55.296875" customWidth="1"/>
+    <col min="24" max="24" width="43.796875" customWidth="1"/>
+    <col min="25" max="25" width="40.19921875" customWidth="1"/>
+    <col min="26" max="26" width="37.296875" customWidth="1"/>
+    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.296875" customWidth="1"/>
+    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.19921875" customWidth="1"/>
+    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="56.296875" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.83203125" customWidth="1"/>
-    <col min="35" max="35" width="45.6640625" customWidth="1"/>
-    <col min="36" max="36" width="39.1640625" customWidth="1"/>
+    <col min="34" max="34" width="58.796875" customWidth="1"/>
+    <col min="35" max="35" width="45.69921875" customWidth="1"/>
+    <col min="36" max="36" width="39.19921875" customWidth="1"/>
     <col min="37" max="37" width="40" customWidth="1"/>
-    <col min="38" max="38" width="41.83203125" customWidth="1"/>
-    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="41.796875" customWidth="1"/>
+    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.83203125" customWidth="1"/>
-    <col min="43" max="43" width="59.6640625" customWidth="1"/>
-    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.796875" customWidth="1"/>
+    <col min="43" max="43" width="59.69921875" customWidth="1"/>
+    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -11185,7 +11320,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="180" customFormat="1" ht="68">
+    <row r="3" spans="1:45" s="180" customFormat="1" ht="62.4">
       <c r="A3" s="151" t="s">
         <v>776</v>
       </c>
@@ -12893,7 +13028,7 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="16" spans="1:45" s="4" customFormat="1" ht="85">
+    <row r="16" spans="1:45" s="4" customFormat="1" ht="78">
       <c r="A16" s="36" t="s">
         <v>2</v>
       </c>
@@ -13014,25 +13149,25 @@
         <v>741</v>
       </c>
     </row>
-    <row r="18" spans="1:45" s="123" customFormat="1" ht="68">
+    <row r="18" spans="1:45" s="123" customFormat="1" ht="62.4">
       <c r="A18" s="159" t="s">
         <v>138</v>
       </c>
       <c r="B18" s="160"/>
       <c r="C18" s="161" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D18" s="161"/>
       <c r="E18" s="162"/>
       <c r="F18" s="162" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G18" s="166" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="H18" s="162"/>
       <c r="I18" s="163" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J18" s="162"/>
       <c r="K18" s="162"/>
@@ -13041,18 +13176,18 @@
       <c r="N18" s="162"/>
       <c r="O18" s="162"/>
       <c r="P18" s="163" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="Q18" s="163" t="s">
         <v>757</v>
       </c>
       <c r="R18" s="163"/>
       <c r="S18" s="163" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T18" s="163"/>
       <c r="U18" s="163" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="V18" s="163"/>
       <c r="W18" s="163" t="s">
@@ -13060,37 +13195,37 @@
       </c>
       <c r="X18" s="163"/>
       <c r="Y18" s="163" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="Z18" s="163"/>
       <c r="AA18" s="163"/>
       <c r="AB18" s="163"/>
       <c r="AC18" s="163" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="AD18" s="163" t="s">
+        <v>844</v>
+      </c>
+      <c r="AE18" s="163" t="s">
         <v>845</v>
-      </c>
-      <c r="AE18" s="163" t="s">
-        <v>846</v>
       </c>
       <c r="AF18" s="163"/>
       <c r="AG18" s="163" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="AH18" s="163"/>
       <c r="AI18" s="163"/>
       <c r="AJ18" s="163" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="AK18" s="163" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="AL18" s="164"/>
       <c r="AM18" s="164"/>
       <c r="AN18" s="164"/>
       <c r="AO18" s="163" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AP18" s="164"/>
       <c r="AQ18" s="164"/>
@@ -13259,16 +13394,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A63FEDD-1574-124C-AE5E-B9EB3BB8513B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="165.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13285,58 +13420,58 @@
         <v>824</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="176" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="51">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="46.8">
       <c r="A4" s="176" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="51">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="46.8">
       <c r="A5" s="176" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="176"/>
       <c r="B6" s="135"/>
     </row>
-    <row r="7" spans="1:2" ht="34">
+    <row r="7" spans="1:2" ht="31.2">
       <c r="A7" s="176" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="176"/>
       <c r="B8" s="135"/>
     </row>
-    <row r="9" spans="1:2" ht="34">
+    <row r="9" spans="1:2" ht="31.2">
       <c r="A9" s="177" t="s">
         <v>704</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="34">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="31.2">
       <c r="A10" s="177" t="s">
         <v>705</v>
       </c>
@@ -13344,12 +13479,12 @@
         <v>707</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="51">
+    <row r="11" spans="1:2" ht="46.8">
       <c r="A11" s="177" t="s">
         <v>706</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="33" customHeight="1">
@@ -13357,7 +13492,7 @@
         <v>725</v>
       </c>
       <c r="B12" s="135" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -13368,7 +13503,7 @@
         <v>758</v>
       </c>
       <c r="B14" s="178" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix: commercial admin level for Germany corrected to 2 in sources file
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\GFZ_local\SERA\From_EFEHR_GitLab\esrm20_exposure\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADEF985-6649-3742-A5F6-2761B42066CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="504" yWindow="516" windowWidth="28296" windowHeight="16704"/>
+    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="COM" sheetId="2" r:id="rId4"/>
     <sheet name="References" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2955,10 +2956,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -3263,7 +3264,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3633,7 +3634,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3738,38 +3739,38 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4086,65 +4087,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="155.69921875" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="155.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="193" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="184"/>
-    </row>
-    <row r="2" spans="1:3" ht="22.05" customHeight="1">
-      <c r="A2" s="186" t="s">
+      <c r="B1" s="193"/>
+    </row>
+    <row r="2" spans="1:3" ht="22" customHeight="1">
+      <c r="A2" s="189" t="s">
         <v>907</v>
       </c>
-      <c r="B2" s="186"/>
+      <c r="B2" s="189"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="22.05" customHeight="1">
-      <c r="A3" s="188" t="s">
+    <row r="3" spans="1:3" ht="22" customHeight="1">
+      <c r="A3" s="190" t="s">
         <v>909</v>
       </c>
-      <c r="B3" s="186"/>
-    </row>
-    <row r="4" spans="1:3" ht="22.05" customHeight="1">
-      <c r="A4" s="186" t="s">
+      <c r="B3" s="189"/>
+    </row>
+    <row r="4" spans="1:3" ht="22" customHeight="1">
+      <c r="A4" s="189" t="s">
         <v>889</v>
       </c>
-      <c r="B4" s="186"/>
-    </row>
-    <row r="5" spans="1:3" ht="22.05" customHeight="1">
-      <c r="A5" s="186" t="s">
+      <c r="B4" s="189"/>
+    </row>
+    <row r="5" spans="1:3" ht="22" customHeight="1">
+      <c r="A5" s="189" t="s">
         <v>908</v>
       </c>
-      <c r="B5" s="186"/>
+      <c r="B5" s="189"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="185"/>
-      <c r="B6" s="185"/>
-    </row>
-    <row r="7" spans="1:3" ht="38.4">
-      <c r="A7" s="189" t="s">
+      <c r="A6" s="194"/>
+      <c r="B6" s="194"/>
+    </row>
+    <row r="7" spans="1:3" ht="39">
+      <c r="A7" s="191" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="191"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="190" t="s">
+      <c r="A8" s="192" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="190"/>
+      <c r="B8" s="192"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4376,50 +4377,50 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="191" t="s">
+      <c r="A40" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B40" s="191"/>
-    </row>
-    <row r="42" spans="1:2" ht="46.8">
+      <c r="B40" s="188"/>
+    </row>
+    <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
         <v>830</v>
       </c>
-      <c r="B42" s="193" t="s">
+      <c r="B42" s="185" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="192" t="s">
+      <c r="A43" s="184" t="s">
         <v>925</v>
       </c>
-      <c r="B43" s="194">
+      <c r="B43" s="186">
         <v>0.3</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="192" t="s">
+      <c r="A44" s="184" t="s">
         <v>926</v>
       </c>
-      <c r="B44" s="194">
+      <c r="B44" s="186">
         <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="192" t="s">
+      <c r="A45" s="184" t="s">
         <v>927</v>
       </c>
-      <c r="B45" s="194">
+      <c r="B45" s="186">
         <v>0.2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="191" t="s">
+      <c r="A47" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B47" s="191"/>
-    </row>
-    <row r="49" spans="1:2" ht="31.2">
+      <c r="B47" s="188"/>
+    </row>
+    <row r="49" spans="1:2" ht="34">
       <c r="A49" s="8" t="s">
         <v>857</v>
       </c>
@@ -4427,17 +4428,17 @@
         <v>897</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="38.4">
-      <c r="A51" s="189" t="s">
+    <row r="51" spans="1:2" ht="39">
+      <c r="A51" s="191" t="s">
         <v>855</v>
       </c>
-      <c r="B51" s="189"/>
+      <c r="B51" s="191"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="190" t="s">
+      <c r="A52" s="192" t="s">
         <v>447</v>
       </c>
-      <c r="B52" s="190"/>
+      <c r="B52" s="192"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3"/>
@@ -4552,12 +4553,12 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="191" t="s">
+      <c r="A70" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B70" s="191"/>
-    </row>
-    <row r="72" spans="1:2" ht="46.8">
+      <c r="B70" s="188"/>
+    </row>
+    <row r="72" spans="1:2" ht="51">
       <c r="A72" s="61" t="s">
         <v>830</v>
       </c>
@@ -4566,36 +4567,36 @@
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="192" t="s">
+      <c r="A73" s="184" t="s">
         <v>925</v>
       </c>
-      <c r="B73" s="194">
+      <c r="B73" s="186">
         <v>0.15</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="192" t="s">
+      <c r="A74" s="184" t="s">
         <v>926</v>
       </c>
-      <c r="B74" s="194">
+      <c r="B74" s="186">
         <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="192" t="s">
+      <c r="A75" s="184" t="s">
         <v>927</v>
       </c>
-      <c r="B75" s="194">
+      <c r="B75" s="186">
         <v>0.6</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="191" t="s">
+      <c r="A77" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B77" s="191"/>
-    </row>
-    <row r="79" spans="1:2" ht="31.2">
+      <c r="B77" s="188"/>
+    </row>
+    <row r="79" spans="1:2" ht="34">
       <c r="A79" s="8" t="s">
         <v>857</v>
       </c>
@@ -4603,23 +4604,23 @@
         <v>898</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="38.4">
-      <c r="A81" s="189" t="s">
+    <row r="81" spans="1:2" ht="39">
+      <c r="A81" s="191" t="s">
         <v>854</v>
       </c>
-      <c r="B81" s="189"/>
+      <c r="B81" s="191"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="190" t="s">
+      <c r="A82" s="192" t="s">
         <v>546</v>
       </c>
-      <c r="B82" s="190"/>
+      <c r="B82" s="192"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
     </row>
-    <row r="84" spans="1:2" ht="31.2">
+    <row r="84" spans="1:2" ht="34">
       <c r="A84" s="151" t="s">
         <v>776</v>
       </c>
@@ -4738,12 +4739,12 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="191" t="s">
+      <c r="A101" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B101" s="191"/>
-    </row>
-    <row r="103" spans="1:2" ht="46.8">
+      <c r="B101" s="188"/>
+    </row>
+    <row r="103" spans="1:2" ht="51">
       <c r="A103" s="61" t="s">
         <v>830</v>
       </c>
@@ -4752,36 +4753,36 @@
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="192" t="s">
+      <c r="A104" s="184" t="s">
         <v>925</v>
       </c>
-      <c r="B104" s="194">
+      <c r="B104" s="186">
         <v>0.2</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="192" t="s">
+      <c r="A105" s="184" t="s">
         <v>926</v>
       </c>
-      <c r="B105" s="194">
+      <c r="B105" s="186">
         <v>0.3</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="192" t="s">
+      <c r="A106" s="184" t="s">
         <v>927</v>
       </c>
-      <c r="B106" s="194">
+      <c r="B106" s="186">
         <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="191" t="s">
+      <c r="A108" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B108" s="191"/>
-    </row>
-    <row r="110" spans="1:2" ht="31.2">
+      <c r="B108" s="188"/>
+    </row>
+    <row r="110" spans="1:2" ht="34">
       <c r="A110" s="8" t="s">
         <v>857</v>
       </c>
@@ -4795,7 +4796,7 @@
       </c>
       <c r="B112" s="187"/>
     </row>
-    <row r="114" spans="1:2" ht="31.2" customHeight="1">
+    <row r="114" spans="1:2" ht="31.25" customHeight="1">
       <c r="A114" s="61" t="s">
         <v>4</v>
       </c>
@@ -4805,6 +4806,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A101:B101"/>
@@ -4820,12 +4827,6 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4833,7 +4834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4843,55 +4844,55 @@
       <selection pane="bottomRight" activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41" style="28" customWidth="1"/>
-    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.296875" customWidth="1"/>
-    <col min="7" max="7" width="61.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" customWidth="1"/>
+    <col min="7" max="7" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" customWidth="1"/>
     <col min="16" max="16" width="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="37.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="37" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.796875" customWidth="1"/>
+    <col min="20" max="20" width="35.83203125" customWidth="1"/>
     <col min="21" max="21" width="36" customWidth="1"/>
-    <col min="22" max="22" width="34.796875" customWidth="1"/>
+    <col min="22" max="22" width="34.83203125" customWidth="1"/>
     <col min="23" max="23" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.796875" customWidth="1"/>
-    <col min="25" max="25" width="40.19921875" customWidth="1"/>
-    <col min="26" max="26" width="37.296875" customWidth="1"/>
-    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.296875" customWidth="1"/>
-    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.19921875" customWidth="1"/>
-    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.83203125" customWidth="1"/>
+    <col min="25" max="25" width="40.1640625" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" customWidth="1"/>
+    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.33203125" customWidth="1"/>
+    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.1640625" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="39.69921875" customWidth="1"/>
-    <col min="35" max="35" width="45.69921875" customWidth="1"/>
-    <col min="36" max="36" width="40.69921875" customWidth="1"/>
-    <col min="37" max="37" width="55.19921875" customWidth="1"/>
-    <col min="38" max="38" width="41.796875" customWidth="1"/>
-    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="39.6640625" customWidth="1"/>
+    <col min="35" max="35" width="45.6640625" customWidth="1"/>
+    <col min="36" max="36" width="40.6640625" customWidth="1"/>
+    <col min="37" max="37" width="55.1640625" customWidth="1"/>
+    <col min="38" max="38" width="41.83203125" customWidth="1"/>
+    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.796875" customWidth="1"/>
-    <col min="43" max="43" width="59.69921875" customWidth="1"/>
-    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.83203125" customWidth="1"/>
+    <col min="43" max="43" width="59.6640625" customWidth="1"/>
+    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -5028,7 +5029,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="2" spans="1:45" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>38</v>
       </c>
@@ -5488,7 +5489,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="46.8">
+    <row r="6" spans="1:45" ht="51">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -5762,7 +5763,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="31.2">
+    <row r="8" spans="1:45" ht="34">
       <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
@@ -6447,7 +6448,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" ht="17">
       <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
@@ -6993,7 +6994,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="17" spans="1:45" ht="190.95" customHeight="1">
+    <row r="17" spans="1:45" ht="191" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>13</v>
       </c>
@@ -7820,7 +7821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:45" ht="140.4">
+    <row r="24" spans="1:45" ht="153">
       <c r="A24" s="25" t="s">
         <v>12</v>
       </c>
@@ -7957,7 +7958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:45" ht="31.2">
+    <row r="25" spans="1:45" ht="34">
       <c r="A25" s="27" t="s">
         <v>2</v>
       </c>
@@ -8229,7 +8230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:45" ht="31.2">
+    <row r="27" spans="1:45" ht="34">
       <c r="A27" s="24" t="s">
         <v>2</v>
       </c>
@@ -8497,7 +8498,7 @@
         <v>22900000</v>
       </c>
     </row>
-    <row r="29" spans="1:45" ht="31.2">
+    <row r="29" spans="1:45" ht="34">
       <c r="A29" s="36" t="s">
         <v>2</v>
       </c>
@@ -8630,7 +8631,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:45" s="4" customFormat="1" ht="130.05000000000001" customHeight="1">
+    <row r="31" spans="1:45" s="4" customFormat="1" ht="130" customHeight="1">
       <c r="A31" s="67" t="s">
         <v>138</v>
       </c>
@@ -8841,9 +8842,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F25" r:id="rId1"/>
-    <hyperlink ref="F27" r:id="rId2"/>
-    <hyperlink ref="F29" r:id="rId3"/>
+    <hyperlink ref="F25" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F27" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F29" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8851,7 +8852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8861,56 +8862,56 @@
       <selection pane="bottomRight" activeCell="AS17" sqref="B17:AS17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
-    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.296875" customWidth="1"/>
-    <col min="4" max="4" width="35.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.5" customWidth="1"/>
-    <col min="8" max="8" width="48.796875" customWidth="1"/>
+    <col min="8" max="8" width="48.83203125" customWidth="1"/>
     <col min="9" max="9" width="43.5" customWidth="1"/>
-    <col min="10" max="10" width="47.796875" customWidth="1"/>
-    <col min="11" max="11" width="46.296875" customWidth="1"/>
-    <col min="12" max="12" width="44.19921875" customWidth="1"/>
-    <col min="13" max="13" width="44.296875" customWidth="1"/>
-    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="47.19921875" customWidth="1"/>
+    <col min="10" max="10" width="47.83203125" customWidth="1"/>
+    <col min="11" max="11" width="46.33203125" customWidth="1"/>
+    <col min="12" max="12" width="44.1640625" customWidth="1"/>
+    <col min="13" max="13" width="44.33203125" customWidth="1"/>
+    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.1640625" customWidth="1"/>
     <col min="16" max="16" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41" customWidth="1"/>
     <col min="20" max="20" width="41.5" customWidth="1"/>
-    <col min="21" max="21" width="43.796875" customWidth="1"/>
-    <col min="22" max="22" width="34.796875" customWidth="1"/>
+    <col min="21" max="21" width="43.83203125" customWidth="1"/>
+    <col min="22" max="22" width="34.83203125" customWidth="1"/>
     <col min="23" max="23" width="39" customWidth="1"/>
-    <col min="24" max="24" width="37.796875" customWidth="1"/>
-    <col min="25" max="25" width="40.19921875" customWidth="1"/>
-    <col min="26" max="26" width="37.296875" customWidth="1"/>
-    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.296875" customWidth="1"/>
-    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.19921875" customWidth="1"/>
-    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.83203125" customWidth="1"/>
+    <col min="25" max="25" width="40.1640625" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" customWidth="1"/>
+    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.33203125" customWidth="1"/>
+    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.1640625" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="39.69921875" customWidth="1"/>
-    <col min="35" max="35" width="45.69921875" customWidth="1"/>
-    <col min="36" max="36" width="39.19921875" customWidth="1"/>
+    <col min="34" max="34" width="39.6640625" customWidth="1"/>
+    <col min="35" max="35" width="45.6640625" customWidth="1"/>
+    <col min="36" max="36" width="39.1640625" customWidth="1"/>
     <col min="37" max="37" width="40" customWidth="1"/>
-    <col min="38" max="38" width="41.796875" customWidth="1"/>
-    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="41.83203125" customWidth="1"/>
+    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.796875" customWidth="1"/>
-    <col min="43" max="43" width="59.69921875" customWidth="1"/>
-    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.83203125" customWidth="1"/>
+    <col min="43" max="43" width="59.6640625" customWidth="1"/>
+    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -9564,7 +9565,7 @@
         <v>201200</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="62.4">
+    <row r="7" spans="1:45" ht="68">
       <c r="A7" s="92" t="s">
         <v>2</v>
       </c>
@@ -9828,7 +9829,7 @@
         <v>201200</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="78">
+    <row r="9" spans="1:45" ht="85">
       <c r="A9" s="103" t="s">
         <v>2</v>
       </c>
@@ -10366,7 +10367,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="13" spans="1:45" s="4" customFormat="1" ht="46.8">
+    <row r="13" spans="1:45" s="4" customFormat="1" ht="51">
       <c r="A13" s="10" t="s">
         <v>712</v>
       </c>
@@ -11051,7 +11052,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="19" spans="1:45" s="123" customFormat="1" ht="31.2">
+    <row r="19" spans="1:45" s="123" customFormat="1" ht="34">
       <c r="A19" s="159" t="s">
         <v>138</v>
       </c>
@@ -11119,66 +11120,66 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.296875" customWidth="1"/>
-    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.296875" customWidth="1"/>
-    <col min="4" max="4" width="47.796875" customWidth="1"/>
-    <col min="5" max="5" width="59.296875" customWidth="1"/>
-    <col min="6" max="6" width="49.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.296875" customWidth="1"/>
-    <col min="8" max="8" width="48.796875" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" customWidth="1"/>
+    <col min="5" max="5" width="59.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.33203125" customWidth="1"/>
+    <col min="8" max="8" width="48.83203125" customWidth="1"/>
     <col min="9" max="9" width="43.5" customWidth="1"/>
-    <col min="10" max="10" width="47.796875" customWidth="1"/>
-    <col min="11" max="11" width="46.296875" customWidth="1"/>
-    <col min="12" max="12" width="44.19921875" customWidth="1"/>
-    <col min="13" max="13" width="44.296875" customWidth="1"/>
-    <col min="14" max="14" width="50.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.83203125" customWidth="1"/>
+    <col min="11" max="11" width="46.33203125" customWidth="1"/>
+    <col min="12" max="12" width="44.1640625" customWidth="1"/>
+    <col min="13" max="13" width="44.33203125" customWidth="1"/>
+    <col min="14" max="14" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="50" customWidth="1"/>
     <col min="16" max="16" width="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="60.796875" customWidth="1"/>
+    <col min="17" max="17" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="60.83203125" customWidth="1"/>
     <col min="19" max="19" width="43.5" customWidth="1"/>
-    <col min="20" max="20" width="49.19921875" customWidth="1"/>
+    <col min="20" max="20" width="49.1640625" customWidth="1"/>
     <col min="21" max="21" width="36" customWidth="1"/>
-    <col min="22" max="22" width="34.796875" customWidth="1"/>
-    <col min="23" max="23" width="55.296875" customWidth="1"/>
-    <col min="24" max="24" width="43.796875" customWidth="1"/>
-    <col min="25" max="25" width="40.19921875" customWidth="1"/>
-    <col min="26" max="26" width="37.296875" customWidth="1"/>
-    <col min="27" max="27" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="51.296875" customWidth="1"/>
-    <col min="29" max="29" width="36.19921875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.19921875" customWidth="1"/>
-    <col min="31" max="31" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="56.296875" customWidth="1"/>
+    <col min="22" max="22" width="34.83203125" customWidth="1"/>
+    <col min="23" max="23" width="55.33203125" customWidth="1"/>
+    <col min="24" max="24" width="43.83203125" customWidth="1"/>
+    <col min="25" max="25" width="40.1640625" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" customWidth="1"/>
+    <col min="27" max="27" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="51.33203125" customWidth="1"/>
+    <col min="29" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.1640625" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="56.33203125" customWidth="1"/>
     <col min="33" max="33" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.796875" customWidth="1"/>
-    <col min="35" max="35" width="45.69921875" customWidth="1"/>
-    <col min="36" max="36" width="39.19921875" customWidth="1"/>
+    <col min="34" max="34" width="58.83203125" customWidth="1"/>
+    <col min="35" max="35" width="45.6640625" customWidth="1"/>
+    <col min="36" max="36" width="39.1640625" customWidth="1"/>
     <col min="37" max="37" width="40" customWidth="1"/>
-    <col min="38" max="38" width="41.796875" customWidth="1"/>
-    <col min="39" max="39" width="46.69921875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="41.83203125" customWidth="1"/>
+    <col min="39" max="39" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="44.5" customWidth="1"/>
     <col min="41" max="41" width="49.5" customWidth="1"/>
-    <col min="42" max="42" width="37.796875" customWidth="1"/>
-    <col min="43" max="43" width="59.69921875" customWidth="1"/>
-    <col min="44" max="44" width="43.296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.83203125" customWidth="1"/>
+    <col min="43" max="43" width="59.6640625" customWidth="1"/>
+    <col min="44" max="44" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="35" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -11320,7 +11321,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="180" customFormat="1" ht="62.4">
+    <row r="3" spans="1:45" s="180" customFormat="1" ht="68">
       <c r="A3" s="151" t="s">
         <v>776</v>
       </c>
@@ -11775,7 +11776,7 @@
         <v>90</v>
       </c>
       <c r="O6" s="94" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="P6" s="94" t="s">
         <v>144</v>
@@ -13028,7 +13029,7 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="16" spans="1:45" s="4" customFormat="1" ht="78">
+    <row r="16" spans="1:45" s="4" customFormat="1" ht="85">
       <c r="A16" s="36" t="s">
         <v>2</v>
       </c>
@@ -13149,7 +13150,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="18" spans="1:45" s="123" customFormat="1" ht="62.4">
+    <row r="18" spans="1:45" s="123" customFormat="1" ht="68">
       <c r="A18" s="159" t="s">
         <v>138</v>
       </c>
@@ -13394,16 +13395,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="165.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13423,7 +13424,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="17">
       <c r="A3" s="176" t="s">
         <v>887</v>
       </c>
@@ -13431,7 +13432,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="46.8">
+    <row r="4" spans="1:2" ht="51">
       <c r="A4" s="176" t="s">
         <v>892</v>
       </c>
@@ -13439,7 +13440,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="46.8">
+    <row r="5" spans="1:2" ht="51">
       <c r="A5" s="176" t="s">
         <v>900</v>
       </c>
@@ -13451,7 +13452,7 @@
       <c r="A6" s="176"/>
       <c r="B6" s="135"/>
     </row>
-    <row r="7" spans="1:2" ht="31.2">
+    <row r="7" spans="1:2" ht="34">
       <c r="A7" s="176" t="s">
         <v>896</v>
       </c>
@@ -13463,7 +13464,7 @@
       <c r="A8" s="176"/>
       <c r="B8" s="135"/>
     </row>
-    <row r="9" spans="1:2" ht="31.2">
+    <row r="9" spans="1:2" ht="34">
       <c r="A9" s="177" t="s">
         <v>704</v>
       </c>
@@ -13471,7 +13472,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="31.2">
+    <row r="10" spans="1:2" ht="34">
       <c r="A10" s="177" t="s">
         <v>705</v>
       </c>
@@ -13479,7 +13480,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="46.8">
+    <row r="11" spans="1:2" ht="51">
       <c r="A11" s="177" t="s">
         <v>706</v>
       </c>

</xml_diff>

<commit_message>
update Swiss residential area and replacement costs based on ERM-CH23
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADEF985-6649-3742-A5F6-2761B42066CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D20F977-E830-0E4B-A614-DE8B1EAEB14E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="520" windowWidth="28300" windowHeight="16700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="28220" windowHeight="16700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="934">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -2951,6 +2951,12 @@
   </si>
   <si>
     <t xml:space="preserve">The structural and non-structural reconstruction cost per m^2 is assumed to comprise 50% of the total replacement cost. The total replacement cost is divided into structural, non-structural and contents according to the percentages shown in the rows below. The structural and non-structural reconstruction cost has been adapted for different materials according to the macro-taxonomy as follows: ﻿MIX:1.00, MUR:0.95, ADO:0.95, CR:1.05, M:1.05, S:1.00, W:0.95, OT:1.00. </t>
+  </si>
+  <si>
+    <t>Earthquake Risk Model of Switzerland ERM-CH23</t>
+  </si>
+  <si>
+    <t>The total floor area has been approximated by taking the volume of buildings in ERM-CH23 and dividing by 3. The reconstruction costs have also been based on average values per m^2 in ERM-CH23</t>
   </si>
 </sst>
 </file>
@@ -3748,6 +3754,15 @@
     <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3755,9 +3770,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3765,12 +3777,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4101,10 +4107,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="187" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="193"/>
+      <c r="B1" s="187"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
       <c r="A2" s="189" t="s">
@@ -4114,7 +4120,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="192" t="s">
         <v>909</v>
       </c>
       <c r="B3" s="189"/>
@@ -4132,20 +4138,20 @@
       <c r="B5" s="189"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="194"/>
-      <c r="B6" s="194"/>
+      <c r="A6" s="188"/>
+      <c r="B6" s="188"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="191" t="s">
+      <c r="A7" s="193" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="191"/>
+      <c r="B7" s="193"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="192" t="s">
+      <c r="A8" s="194" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="192"/>
+      <c r="B8" s="194"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4311,10 +4317,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="187" t="s">
+      <c r="A30" s="190" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="187"/>
+      <c r="B30" s="190"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4377,10 +4383,10 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="188" t="s">
+      <c r="A40" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B40" s="188"/>
+      <c r="B40" s="191"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4415,10 +4421,10 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="188" t="s">
+      <c r="A47" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B47" s="188"/>
+      <c r="B47" s="191"/>
     </row>
     <row r="49" spans="1:2" ht="34">
       <c r="A49" s="8" t="s">
@@ -4429,16 +4435,16 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="39">
-      <c r="A51" s="191" t="s">
+      <c r="A51" s="193" t="s">
         <v>855</v>
       </c>
-      <c r="B51" s="191"/>
+      <c r="B51" s="193"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="192" t="s">
+      <c r="A52" s="194" t="s">
         <v>447</v>
       </c>
-      <c r="B52" s="192"/>
+      <c r="B52" s="194"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3"/>
@@ -4553,10 +4559,10 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="188" t="s">
+      <c r="A70" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B70" s="188"/>
+      <c r="B70" s="191"/>
     </row>
     <row r="72" spans="1:2" ht="51">
       <c r="A72" s="61" t="s">
@@ -4591,10 +4597,10 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="188" t="s">
+      <c r="A77" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B77" s="188"/>
+      <c r="B77" s="191"/>
     </row>
     <row r="79" spans="1:2" ht="34">
       <c r="A79" s="8" t="s">
@@ -4605,16 +4611,16 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="39">
-      <c r="A81" s="191" t="s">
+      <c r="A81" s="193" t="s">
         <v>854</v>
       </c>
-      <c r="B81" s="191"/>
+      <c r="B81" s="193"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="192" t="s">
+      <c r="A82" s="194" t="s">
         <v>546</v>
       </c>
-      <c r="B82" s="192"/>
+      <c r="B82" s="194"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3"/>
@@ -4697,10 +4703,10 @@
       <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="187" t="s">
+      <c r="A94" s="190" t="s">
         <v>212</v>
       </c>
-      <c r="B94" s="187"/>
+      <c r="B94" s="190"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4"/>
@@ -4739,10 +4745,10 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="188" t="s">
+      <c r="A101" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B101" s="188"/>
+      <c r="B101" s="191"/>
     </row>
     <row r="103" spans="1:2" ht="51">
       <c r="A103" s="61" t="s">
@@ -4777,10 +4783,10 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="188" t="s">
+      <c r="A108" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B108" s="188"/>
+      <c r="B108" s="191"/>
     </row>
     <row r="110" spans="1:2" ht="34">
       <c r="A110" s="8" t="s">
@@ -4791,10 +4797,10 @@
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="187" t="s">
+      <c r="A112" s="190" t="s">
         <v>698</v>
       </c>
-      <c r="B112" s="187"/>
+      <c r="B112" s="190"/>
     </row>
     <row r="114" spans="1:2" ht="31.25" customHeight="1">
       <c r="A114" s="61" t="s">
@@ -4806,12 +4812,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A101:B101"/>
@@ -4827,6 +4827,12 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4837,11 +4843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AN17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB32" sqref="AB32"/>
+      <selection pane="bottomRight" activeCell="AQ20" sqref="AQ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -7396,7 +7402,7 @@
         <v>8</v>
       </c>
       <c r="AQ19" s="42">
-        <v>2010</v>
+        <v>2500</v>
       </c>
       <c r="AR19" s="42">
         <v>440</v>
@@ -7533,7 +7539,7 @@
         <v>1550</v>
       </c>
       <c r="AQ20" s="43">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="AR20" s="43">
         <v>320</v>
@@ -7670,7 +7676,7 @@
         <v>1350</v>
       </c>
       <c r="AQ21" s="44">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="AR21" s="44">
         <v>250</v>
@@ -7812,7 +7818,7 @@
         <v>8</v>
       </c>
       <c r="AQ23" s="45">
-        <v>437633270</v>
+        <v>818056531.70000005</v>
       </c>
       <c r="AR23" s="45">
         <v>1192264869</v>
@@ -8086,7 +8092,7 @@
         <v>8</v>
       </c>
       <c r="AQ25" s="32" t="s">
-        <v>283</v>
+        <v>932</v>
       </c>
       <c r="AR25" s="32" t="s">
         <v>286</v>
@@ -8696,7 +8702,9 @@
         <v>852</v>
       </c>
       <c r="AP31" s="170"/>
-      <c r="AQ31" s="170"/>
+      <c r="AQ31" s="172" t="s">
+        <v>933</v>
+      </c>
       <c r="AR31" s="170"/>
       <c r="AS31" s="170"/>
     </row>
@@ -11123,7 +11131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
update industrial building assumptions for Switzerland based on ERM-CH23
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D20F977-E830-0E4B-A614-DE8B1EAEB14E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56B6FD-0BAA-334F-A178-2202BA5A6448}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="28220" windowHeight="16700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="6300" windowWidth="28220" windowHeight="16700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="937">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -2957,6 +2957,15 @@
   </si>
   <si>
     <t>The total floor area has been approximated by taking the volume of buildings in ERM-CH23 and dividing by 3. The reconstruction costs have also been based on average values per m^2 in ERM-CH23</t>
+  </si>
+  <si>
+    <t>ERM-CH23</t>
+  </si>
+  <si>
+    <t>ERM-CH23 based on volume/4.5</t>
+  </si>
+  <si>
+    <t>Reconstruction cost, number and area based on ERM-CH23</t>
   </si>
 </sst>
 </file>
@@ -3754,29 +3763,29 @@
     <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4107,10 +4116,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="193" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="187"/>
+      <c r="B1" s="193"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
       <c r="A2" s="189" t="s">
@@ -4120,7 +4129,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="190" t="s">
         <v>909</v>
       </c>
       <c r="B3" s="189"/>
@@ -4138,20 +4147,20 @@
       <c r="B5" s="189"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="188"/>
-      <c r="B6" s="188"/>
+      <c r="A6" s="194"/>
+      <c r="B6" s="194"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="193" t="s">
+      <c r="A7" s="191" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="193"/>
+      <c r="B7" s="191"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="194" t="s">
+      <c r="A8" s="192" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="194"/>
+      <c r="B8" s="192"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4317,10 +4326,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="190" t="s">
+      <c r="A30" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="190"/>
+      <c r="B30" s="187"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4383,10 +4392,10 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="191" t="s">
+      <c r="A40" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B40" s="191"/>
+      <c r="B40" s="188"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4421,10 +4430,10 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="191" t="s">
+      <c r="A47" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B47" s="191"/>
+      <c r="B47" s="188"/>
     </row>
     <row r="49" spans="1:2" ht="34">
       <c r="A49" s="8" t="s">
@@ -4435,16 +4444,16 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="39">
-      <c r="A51" s="193" t="s">
+      <c r="A51" s="191" t="s">
         <v>855</v>
       </c>
-      <c r="B51" s="193"/>
+      <c r="B51" s="191"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="194" t="s">
+      <c r="A52" s="192" t="s">
         <v>447</v>
       </c>
-      <c r="B52" s="194"/>
+      <c r="B52" s="192"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3"/>
@@ -4559,10 +4568,10 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="191" t="s">
+      <c r="A70" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B70" s="191"/>
+      <c r="B70" s="188"/>
     </row>
     <row r="72" spans="1:2" ht="51">
       <c r="A72" s="61" t="s">
@@ -4597,10 +4606,10 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="191" t="s">
+      <c r="A77" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B77" s="191"/>
+      <c r="B77" s="188"/>
     </row>
     <row r="79" spans="1:2" ht="34">
       <c r="A79" s="8" t="s">
@@ -4611,16 +4620,16 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="39">
-      <c r="A81" s="193" t="s">
+      <c r="A81" s="191" t="s">
         <v>854</v>
       </c>
-      <c r="B81" s="193"/>
+      <c r="B81" s="191"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="194" t="s">
+      <c r="A82" s="192" t="s">
         <v>546</v>
       </c>
-      <c r="B82" s="194"/>
+      <c r="B82" s="192"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3"/>
@@ -4703,10 +4712,10 @@
       <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="190" t="s">
+      <c r="A94" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="B94" s="190"/>
+      <c r="B94" s="187"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4"/>
@@ -4745,10 +4754,10 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="191" t="s">
+      <c r="A101" s="188" t="s">
         <v>929</v>
       </c>
-      <c r="B101" s="191"/>
+      <c r="B101" s="188"/>
     </row>
     <row r="103" spans="1:2" ht="51">
       <c r="A103" s="61" t="s">
@@ -4783,10 +4792,10 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="191" t="s">
+      <c r="A108" s="188" t="s">
         <v>924</v>
       </c>
-      <c r="B108" s="191"/>
+      <c r="B108" s="188"/>
     </row>
     <row r="110" spans="1:2" ht="34">
       <c r="A110" s="8" t="s">
@@ -4797,10 +4806,10 @@
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="190" t="s">
+      <c r="A112" s="187" t="s">
         <v>698</v>
       </c>
-      <c r="B112" s="190"/>
+      <c r="B112" s="187"/>
     </row>
     <row r="114" spans="1:2" ht="31.25" customHeight="1">
       <c r="A114" s="61" t="s">
@@ -4812,6 +4821,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A101:B101"/>
@@ -4827,12 +4842,6 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4843,7 +4852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AN17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8863,11 +8872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AP9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS17" sqref="B17:AS17"/>
+      <selection pane="bottomRight" activeCell="AQ21" sqref="AQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -9828,7 +9837,7 @@
         <v>99350</v>
       </c>
       <c r="AQ8" s="58">
-        <v>25000</v>
+        <v>53066</v>
       </c>
       <c r="AR8" s="58">
         <v>197027</v>
@@ -9965,7 +9974,7 @@
         <v>682</v>
       </c>
       <c r="AQ9" s="106" t="s">
-        <v>461</v>
+        <v>934</v>
       </c>
       <c r="AR9" s="100" t="s">
         <v>285</v>
@@ -10092,7 +10101,7 @@
         <v>132579788.07735008</v>
       </c>
       <c r="AQ10" s="95">
-        <v>48151580.75840807</v>
+        <v>111102462.40000001</v>
       </c>
       <c r="AR10" s="95">
         <v>173029820.63733897</v>
@@ -10229,7 +10238,8 @@
         <v>1334.4719484383502</v>
       </c>
       <c r="AQ11" s="105">
-        <v>1926.0632303363227</v>
+        <f>AQ10/AQ8</f>
+        <v>2093.6656691666981</v>
       </c>
       <c r="AR11" s="104">
         <v>878</v>
@@ -10366,7 +10376,7 @@
         <v>704</v>
       </c>
       <c r="AQ12" s="104" t="s">
-        <v>704</v>
+        <v>935</v>
       </c>
       <c r="AR12" s="104" t="s">
         <v>704</v>
@@ -11051,7 +11061,7 @@
         <v>850</v>
       </c>
       <c r="AQ17" s="126">
-        <v>950</v>
+        <v>1150</v>
       </c>
       <c r="AR17" s="126">
         <v>220</v>
@@ -11113,7 +11123,9 @@
         <v>850</v>
       </c>
       <c r="AP19" s="164"/>
-      <c r="AQ19" s="164"/>
+      <c r="AQ19" s="163" t="s">
+        <v>936</v>
+      </c>
       <c r="AR19" s="165" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
update areas per building (double) to match more closely area in ERM-CH23
</commit_message>
<xml_diff>
--- a/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
+++ b/sources/European_Exposure_Model_Data_Inputs_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56B6FD-0BAA-334F-A178-2202BA5A6448}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8E25E1-885B-2C41-ABAD-2DA77B5E897F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="6300" windowWidth="28220" windowHeight="16700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="28220" windowHeight="16700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="938">
   <si>
     <t>data_Albania_RES_census-buildings.xlsx</t>
   </si>
@@ -2965,7 +2965,10 @@
     <t>ERM-CH23 based on volume/4.5</t>
   </si>
   <si>
-    <t>Reconstruction cost, number and area based on ERM-CH23</t>
+    <t>Number and area based on ERM-CH23</t>
+  </si>
+  <si>
+    <t>Areas per building have been doubled to match more closely the total area of commercial buildings in ERM-CH23</t>
   </si>
 </sst>
 </file>
@@ -3763,6 +3766,15 @@
     <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3770,9 +3782,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3780,12 +3789,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4116,10 +4119,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="187" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="193"/>
+      <c r="B1" s="187"/>
     </row>
     <row r="2" spans="1:3" ht="22" customHeight="1">
       <c r="A2" s="189" t="s">
@@ -4129,7 +4132,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="22" customHeight="1">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="192" t="s">
         <v>909</v>
       </c>
       <c r="B3" s="189"/>
@@ -4147,20 +4150,20 @@
       <c r="B5" s="189"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="194"/>
-      <c r="B6" s="194"/>
+      <c r="A6" s="188"/>
+      <c r="B6" s="188"/>
     </row>
     <row r="7" spans="1:3" ht="39">
-      <c r="A7" s="191" t="s">
+      <c r="A7" s="193" t="s">
         <v>687</v>
       </c>
-      <c r="B7" s="191"/>
+      <c r="B7" s="193"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="192" t="s">
+      <c r="A8" s="194" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="192"/>
+      <c r="B8" s="194"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
@@ -4326,10 +4329,10 @@
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="187" t="s">
+      <c r="A30" s="190" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="187"/>
+      <c r="B30" s="190"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4"/>
@@ -4392,10 +4395,10 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="188" t="s">
+      <c r="A40" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B40" s="188"/>
+      <c r="B40" s="191"/>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="A42" s="61" t="s">
@@ -4430,10 +4433,10 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="188" t="s">
+      <c r="A47" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B47" s="188"/>
+      <c r="B47" s="191"/>
     </row>
     <row r="49" spans="1:2" ht="34">
       <c r="A49" s="8" t="s">
@@ -4444,16 +4447,16 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="39">
-      <c r="A51" s="191" t="s">
+      <c r="A51" s="193" t="s">
         <v>855</v>
       </c>
-      <c r="B51" s="191"/>
+      <c r="B51" s="193"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="192" t="s">
+      <c r="A52" s="194" t="s">
         <v>447</v>
       </c>
-      <c r="B52" s="192"/>
+      <c r="B52" s="194"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3"/>
@@ -4568,10 +4571,10 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="188" t="s">
+      <c r="A70" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B70" s="188"/>
+      <c r="B70" s="191"/>
     </row>
     <row r="72" spans="1:2" ht="51">
       <c r="A72" s="61" t="s">
@@ -4606,10 +4609,10 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="188" t="s">
+      <c r="A77" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B77" s="188"/>
+      <c r="B77" s="191"/>
     </row>
     <row r="79" spans="1:2" ht="34">
       <c r="A79" s="8" t="s">
@@ -4620,16 +4623,16 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="39">
-      <c r="A81" s="191" t="s">
+      <c r="A81" s="193" t="s">
         <v>854</v>
       </c>
-      <c r="B81" s="191"/>
+      <c r="B81" s="193"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="192" t="s">
+      <c r="A82" s="194" t="s">
         <v>546</v>
       </c>
-      <c r="B82" s="192"/>
+      <c r="B82" s="194"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3"/>
@@ -4712,10 +4715,10 @@
       <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="187" t="s">
+      <c r="A94" s="190" t="s">
         <v>212</v>
       </c>
-      <c r="B94" s="187"/>
+      <c r="B94" s="190"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4"/>
@@ -4754,10 +4757,10 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="188" t="s">
+      <c r="A101" s="191" t="s">
         <v>929</v>
       </c>
-      <c r="B101" s="188"/>
+      <c r="B101" s="191"/>
     </row>
     <row r="103" spans="1:2" ht="51">
       <c r="A103" s="61" t="s">
@@ -4792,10 +4795,10 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="188" t="s">
+      <c r="A108" s="191" t="s">
         <v>924</v>
       </c>
-      <c r="B108" s="188"/>
+      <c r="B108" s="191"/>
     </row>
     <row r="110" spans="1:2" ht="34">
       <c r="A110" s="8" t="s">
@@ -4806,10 +4809,10 @@
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="187" t="s">
+      <c r="A112" s="190" t="s">
         <v>698</v>
       </c>
-      <c r="B112" s="187"/>
+      <c r="B112" s="190"/>
     </row>
     <row r="114" spans="1:2" ht="31.25" customHeight="1">
       <c r="A114" s="61" t="s">
@@ -4821,12 +4824,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A101:B101"/>
@@ -4842,6 +4839,12 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8872,11 +8875,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AP9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ21" sqref="AQ21"/>
+      <selection pane="bottomRight" activeCell="AQ19" sqref="AQ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -11143,11 +11146,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="AQ17" sqref="AQ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -13249,7 +13252,9 @@
         <v>849</v>
       </c>
       <c r="AP18" s="164"/>
-      <c r="AQ18" s="164"/>
+      <c r="AQ18" s="163" t="s">
+        <v>937</v>
+      </c>
       <c r="AR18" s="165" t="s">
         <v>8</v>
       </c>

</xml_diff>